<commit_message>
Feitos testes para a tabela 1 e o código para facilitar a cópia de dados para o Excel
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="19920" windowHeight="8010" tabRatio="338"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="19920" windowHeight="8010" tabRatio="338" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Abcissas fixas" sheetId="1" r:id="rId1"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1166,22 +1166,54 @@
       <c r="D4" s="13">
         <v>20</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6"/>
+      <c r="E4" s="4">
+        <v>7.0217499999999999</v>
+      </c>
+      <c r="F4" s="5">
+        <v>7.67896</v>
+      </c>
+      <c r="G4" s="5">
+        <v>7.0705</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0.11092</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1.659</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.8543700000000001</v>
+      </c>
+      <c r="K4" s="5">
+        <v>1.75641</v>
+      </c>
+      <c r="L4" s="21">
+        <v>7.4899999999999994E-2</v>
+      </c>
+      <c r="M4" s="4">
+        <v>6.2221000000000002</v>
+      </c>
+      <c r="N4" s="5">
+        <v>6.8118499999999997</v>
+      </c>
+      <c r="O4" s="5">
+        <v>6.5476200000000002</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0.14741000000000001</v>
+      </c>
+      <c r="Q4" s="17">
+        <v>7.4272099999999996</v>
+      </c>
+      <c r="R4" s="5">
+        <v>7.6356599999999997</v>
+      </c>
+      <c r="S4" s="5">
+        <v>7.6150000000000002</v>
+      </c>
+      <c r="T4" s="6">
+        <v>3.8469999999999997E-2</v>
+      </c>
     </row>
     <row r="5" spans="2:20">
       <c r="B5" s="40"/>
@@ -1189,22 +1221,54 @@
       <c r="D5" s="14">
         <v>50</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="T5" s="9"/>
+      <c r="E5" s="7">
+        <v>5.0242199999999997</v>
+      </c>
+      <c r="F5" s="8">
+        <v>5.0442999999999998</v>
+      </c>
+      <c r="G5" s="8">
+        <v>5.0360300000000002</v>
+      </c>
+      <c r="H5" s="9">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1.6759599999999999</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1.78295</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1.7721</v>
+      </c>
+      <c r="L5" s="22">
+        <v>2.8629999999999999E-2</v>
+      </c>
+      <c r="M5" s="7">
+        <v>4.8667600000000002</v>
+      </c>
+      <c r="N5" s="8">
+        <v>4.8671100000000003</v>
+      </c>
+      <c r="O5" s="8">
+        <v>4.8669200000000004</v>
+      </c>
+      <c r="P5" s="9">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>7.4568199999999996</v>
+      </c>
+      <c r="R5" s="8">
+        <v>7.5282400000000003</v>
+      </c>
+      <c r="S5" s="8">
+        <v>7.50732</v>
+      </c>
+      <c r="T5" s="9">
+        <v>2.0330000000000001E-2</v>
+      </c>
     </row>
     <row r="6" spans="2:20">
       <c r="B6" s="40"/>
@@ -1214,22 +1278,54 @@
       <c r="D6" s="14">
         <v>100</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="9"/>
+      <c r="E6" s="7">
+        <v>5.1773999999999996</v>
+      </c>
+      <c r="F6" s="8">
+        <v>5.3295700000000004</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5.18757</v>
+      </c>
+      <c r="H6" s="9">
+        <v>2.3650000000000001E-2</v>
+      </c>
+      <c r="I6" s="18">
+        <v>1.6420999999999999</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1.64225</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.64225</v>
+      </c>
+      <c r="L6" s="22">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="M6" s="7">
+        <v>4.9325299999999999</v>
+      </c>
+      <c r="N6" s="8">
+        <v>5.8435699999999997</v>
+      </c>
+      <c r="O6" s="8">
+        <v>4.9901499999999999</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0.2059</v>
+      </c>
+      <c r="Q6" s="18">
+        <v>7.1666699999999999</v>
+      </c>
+      <c r="R6" s="8">
+        <v>7.1884300000000003</v>
+      </c>
+      <c r="S6" s="8">
+        <v>7.1849499999999997</v>
+      </c>
+      <c r="T6" s="9">
+        <v>7.9799999999999992E-3</v>
+      </c>
     </row>
     <row r="7" spans="2:20" ht="15.75" thickBot="1">
       <c r="B7" s="40"/>
@@ -1237,22 +1333,54 @@
       <c r="D7" s="29">
         <v>250</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="26"/>
+      <c r="E7" s="24">
+        <v>4.5209799999999998</v>
+      </c>
+      <c r="F7" s="25">
+        <v>4.5209799999999998</v>
+      </c>
+      <c r="G7" s="25">
+        <v>4.5209799999999998</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27">
+        <v>1.22153</v>
+      </c>
+      <c r="J7" s="25">
+        <v>1.2268300000000001</v>
+      </c>
+      <c r="K7" s="25">
+        <v>1.22672</v>
+      </c>
+      <c r="L7" s="28">
+        <v>7.3999999999999999E-4</v>
+      </c>
+      <c r="M7" s="24">
+        <v>4.31149</v>
+      </c>
+      <c r="N7" s="25">
+        <v>4.3115500000000004</v>
+      </c>
+      <c r="O7" s="25">
+        <v>4.3115199999999998</v>
+      </c>
+      <c r="P7" s="26">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>7.0185000000000004</v>
+      </c>
+      <c r="R7" s="25">
+        <v>7.0185000000000004</v>
+      </c>
+      <c r="S7" s="25">
+        <v>7.0185000000000004</v>
+      </c>
+      <c r="T7" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:20">
       <c r="B8" s="40"/>
@@ -1260,22 +1388,54 @@
       <c r="D8" s="13">
         <v>20</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="6"/>
+      <c r="E8" s="4">
+        <v>5.1893399999999996</v>
+      </c>
+      <c r="F8" s="5">
+        <v>5.8871500000000001</v>
+      </c>
+      <c r="G8" s="5">
+        <v>5.4970400000000001</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.12304</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1.74505</v>
+      </c>
+      <c r="J8" s="5">
+        <v>2.0032199999999998</v>
+      </c>
+      <c r="K8" s="5">
+        <v>1.87459</v>
+      </c>
+      <c r="L8" s="21">
+        <v>4.0629999999999999E-2</v>
+      </c>
+      <c r="M8" s="4">
+        <v>4.7875899999999998</v>
+      </c>
+      <c r="N8" s="5">
+        <v>5.5719200000000004</v>
+      </c>
+      <c r="O8" s="5">
+        <v>5.2586899999999996</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0.15315999999999999</v>
+      </c>
+      <c r="Q8" s="17">
+        <v>7.61287</v>
+      </c>
+      <c r="R8" s="5">
+        <v>7.6792800000000003</v>
+      </c>
+      <c r="S8" s="5">
+        <v>7.6401700000000003</v>
+      </c>
+      <c r="T8" s="6">
+        <v>1.566E-2</v>
+      </c>
     </row>
     <row r="9" spans="2:20">
       <c r="B9" s="40"/>
@@ -1283,22 +1443,54 @@
       <c r="D9" s="14">
         <v>50</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="9"/>
+      <c r="E9" s="7">
+        <v>4.6554399999999996</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4.6812800000000001</v>
+      </c>
+      <c r="G9" s="8">
+        <v>4.6703900000000003</v>
+      </c>
+      <c r="H9" s="9">
+        <v>6.7099999999999998E-3</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1.3787499999999999</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1.3817200000000001</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1.3804399999999999</v>
+      </c>
+      <c r="L9" s="22">
+        <v>9.7000000000000005E-4</v>
+      </c>
+      <c r="M9" s="7">
+        <v>4.4266399999999999</v>
+      </c>
+      <c r="N9" s="8">
+        <v>4.4804399999999998</v>
+      </c>
+      <c r="O9" s="8">
+        <v>4.4396300000000002</v>
+      </c>
+      <c r="P9" s="9">
+        <v>2.2929999999999999E-2</v>
+      </c>
+      <c r="Q9" s="18">
+        <v>7.1420599999999999</v>
+      </c>
+      <c r="R9" s="8">
+        <v>7.1450699999999996</v>
+      </c>
+      <c r="S9" s="8">
+        <v>7.1443399999999997</v>
+      </c>
+      <c r="T9" s="9">
+        <v>8.0000000000000004E-4</v>
+      </c>
     </row>
     <row r="10" spans="2:20">
       <c r="B10" s="40"/>
@@ -1308,22 +1500,54 @@
       <c r="D10" s="14">
         <v>100</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="9"/>
+      <c r="E10" s="7">
+        <v>3.9096500000000001</v>
+      </c>
+      <c r="F10" s="8">
+        <v>4.5678000000000001</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3.9162300000000001</v>
+      </c>
+      <c r="H10" s="9">
+        <v>6.5490000000000007E-2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>1.5398799999999999</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1.5398799999999999</v>
+      </c>
+      <c r="K10" s="8">
+        <v>1.5398799999999999</v>
+      </c>
+      <c r="L10" s="22">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>4.3118699999999999</v>
+      </c>
+      <c r="N10" s="8">
+        <v>4.3703599999999998</v>
+      </c>
+      <c r="O10" s="8">
+        <v>4.31663</v>
+      </c>
+      <c r="P10" s="9">
+        <v>1.584E-2</v>
+      </c>
+      <c r="Q10" s="18">
+        <v>7.0376500000000002</v>
+      </c>
+      <c r="R10" s="8">
+        <v>7.2181600000000001</v>
+      </c>
+      <c r="S10" s="8">
+        <v>7.0456399999999997</v>
+      </c>
+      <c r="T10" s="9">
+        <v>2.009E-2</v>
+      </c>
     </row>
     <row r="11" spans="2:20" ht="15.75" thickBot="1">
       <c r="B11" s="40">
@@ -1333,22 +1557,54 @@
       <c r="D11" s="29">
         <v>250</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="26"/>
+      <c r="E11" s="24">
+        <v>4.8247600000000004</v>
+      </c>
+      <c r="F11" s="25">
+        <v>4.8266600000000004</v>
+      </c>
+      <c r="G11" s="25">
+        <v>4.8261099999999999</v>
+      </c>
+      <c r="H11" s="26">
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="I11" s="27">
+        <v>1.2935000000000001</v>
+      </c>
+      <c r="J11" s="25">
+        <v>1.32605</v>
+      </c>
+      <c r="K11" s="25">
+        <v>1.2946</v>
+      </c>
+      <c r="L11" s="28">
+        <v>3.49E-3</v>
+      </c>
+      <c r="M11" s="24">
+        <v>4.3110999999999997</v>
+      </c>
+      <c r="N11" s="25">
+        <v>4.4495800000000001</v>
+      </c>
+      <c r="O11" s="25">
+        <v>4.3149100000000002</v>
+      </c>
+      <c r="P11" s="26">
+        <v>2.0740000000000001E-2</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>7.0145900000000001</v>
+      </c>
+      <c r="R11" s="25">
+        <v>7.0145900000000001</v>
+      </c>
+      <c r="S11" s="25">
+        <v>7.0145900000000001</v>
+      </c>
+      <c r="T11" s="26">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:20">
       <c r="B12" s="40"/>
@@ -1356,22 +1612,54 @@
       <c r="D12" s="13">
         <v>20</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
+      <c r="E12" s="4">
+        <v>5.21706</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5.8344899999999997</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5.6711600000000004</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.10015</v>
+      </c>
+      <c r="I12" s="17">
+        <v>1.67645</v>
+      </c>
+      <c r="J12" s="5">
+        <v>1.74535</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1.6934199999999999</v>
+      </c>
+      <c r="L12" s="21">
+        <v>8.4499999999999992E-3</v>
+      </c>
+      <c r="M12" s="4">
+        <v>4.8465499999999997</v>
+      </c>
+      <c r="N12" s="5">
+        <v>5.1000500000000004</v>
+      </c>
+      <c r="O12" s="5">
+        <v>4.9393099999999999</v>
+      </c>
+      <c r="P12" s="6">
+        <v>5.1670000000000001E-2</v>
+      </c>
+      <c r="Q12" s="17">
+        <v>7.2526799999999998</v>
+      </c>
+      <c r="R12" s="5">
+        <v>7.3491799999999996</v>
+      </c>
+      <c r="S12" s="5">
+        <v>7.3292400000000004</v>
+      </c>
+      <c r="T12" s="6">
+        <v>1.453E-2</v>
+      </c>
     </row>
     <row r="13" spans="2:20">
       <c r="B13" s="40"/>
@@ -1379,22 +1667,54 @@
       <c r="D13" s="14">
         <v>50</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="9"/>
+      <c r="E13" s="7">
+        <v>5.5274299999999998</v>
+      </c>
+      <c r="F13" s="8">
+        <v>5.5742200000000004</v>
+      </c>
+      <c r="G13" s="8">
+        <v>5.5432699999999997</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1.1429999999999999E-2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1.2168300000000001</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1.2483900000000001</v>
+      </c>
+      <c r="K13" s="8">
+        <v>1.24396</v>
+      </c>
+      <c r="L13" s="22">
+        <v>4.3E-3</v>
+      </c>
+      <c r="M13" s="7">
+        <v>4.3486399999999996</v>
+      </c>
+      <c r="N13" s="8">
+        <v>4.3614199999999999</v>
+      </c>
+      <c r="O13" s="8">
+        <v>4.3595100000000002</v>
+      </c>
+      <c r="P13" s="9">
+        <v>4.4600000000000004E-3</v>
+      </c>
+      <c r="Q13" s="18">
+        <v>7.1189999999999998</v>
+      </c>
+      <c r="R13" s="8">
+        <v>7.1297100000000002</v>
+      </c>
+      <c r="S13" s="8">
+        <v>7.1264200000000004</v>
+      </c>
+      <c r="T13" s="9">
+        <v>1.0499999999999999E-3</v>
+      </c>
     </row>
     <row r="14" spans="2:20">
       <c r="B14" s="40"/>
@@ -1404,22 +1724,54 @@
       <c r="D14" s="14">
         <v>100</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="9"/>
+      <c r="E14" s="7">
+        <v>3.8160599999999998</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3.8233600000000001</v>
+      </c>
+      <c r="G14" s="8">
+        <v>3.8220999999999998</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1.0499999999999999E-3</v>
+      </c>
+      <c r="I14" s="18">
+        <v>1.1932499999999999</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1.1952199999999999</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1.19458</v>
+      </c>
+      <c r="L14" s="22">
+        <v>2.9E-4</v>
+      </c>
+      <c r="M14" s="7">
+        <v>4.3074899999999996</v>
+      </c>
+      <c r="N14" s="8">
+        <v>4.3074899999999996</v>
+      </c>
+      <c r="O14" s="8">
+        <v>4.3074899999999996</v>
+      </c>
+      <c r="P14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="18">
+        <v>7.0225600000000004</v>
+      </c>
+      <c r="R14" s="8">
+        <v>7.0278999999999998</v>
+      </c>
+      <c r="S14" s="8">
+        <v>7.0277500000000002</v>
+      </c>
+      <c r="T14" s="9">
+        <v>8.3000000000000001E-4</v>
+      </c>
     </row>
     <row r="15" spans="2:20" ht="15.75" thickBot="1">
       <c r="B15" s="40"/>
@@ -1427,22 +1779,54 @@
       <c r="D15" s="29">
         <v>250</v>
       </c>
-      <c r="E15" s="24"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="26"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="26"/>
+      <c r="E15" s="24">
+        <v>3.7760600000000002</v>
+      </c>
+      <c r="F15" s="25">
+        <v>3.7765200000000001</v>
+      </c>
+      <c r="G15" s="25">
+        <v>3.77651</v>
+      </c>
+      <c r="H15" s="26">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="I15" s="27">
+        <v>1.25996</v>
+      </c>
+      <c r="J15" s="25">
+        <v>1.36253</v>
+      </c>
+      <c r="K15" s="25">
+        <v>1.2659199999999999</v>
+      </c>
+      <c r="L15" s="28">
+        <v>9.6900000000000007E-3</v>
+      </c>
+      <c r="M15" s="24">
+        <v>4.3055599999999998</v>
+      </c>
+      <c r="N15" s="25">
+        <v>4.3055700000000003</v>
+      </c>
+      <c r="O15" s="25">
+        <v>4.3055700000000003</v>
+      </c>
+      <c r="P15" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>7.0038</v>
+      </c>
+      <c r="R15" s="25">
+        <v>7.00474</v>
+      </c>
+      <c r="S15" s="25">
+        <v>7.0042499999999999</v>
+      </c>
+      <c r="T15" s="26">
+        <v>6.0000000000000002E-5</v>
+      </c>
     </row>
     <row r="16" spans="2:20">
       <c r="B16" s="40"/>
@@ -1450,22 +1834,54 @@
       <c r="D16" s="13">
         <v>20</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="17"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="6"/>
+      <c r="E16" s="4">
+        <v>4.0557100000000004</v>
+      </c>
+      <c r="F16" s="5">
+        <v>5.3661300000000001</v>
+      </c>
+      <c r="G16" s="5">
+        <v>4.63293</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.28149999999999997</v>
+      </c>
+      <c r="I16" s="17">
+        <v>1.39608</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.72888</v>
+      </c>
+      <c r="K16" s="5">
+        <v>1.5276000000000001</v>
+      </c>
+      <c r="L16" s="21">
+        <v>6.2280000000000002E-2</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4.4506199999999998</v>
+      </c>
+      <c r="N16" s="5">
+        <v>5.5277700000000003</v>
+      </c>
+      <c r="O16" s="5">
+        <v>4.8948299999999998</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0.14130999999999999</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>7.1368499999999999</v>
+      </c>
+      <c r="R16" s="5">
+        <v>7.2453200000000004</v>
+      </c>
+      <c r="S16" s="5">
+        <v>7.2051999999999996</v>
+      </c>
+      <c r="T16" s="6">
+        <v>1.374E-2</v>
+      </c>
     </row>
     <row r="17" spans="2:20">
       <c r="B17" s="40"/>
@@ -1473,22 +1889,54 @@
       <c r="D17" s="14">
         <v>50</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="9"/>
+      <c r="E17" s="7">
+        <v>3.9236599999999999</v>
+      </c>
+      <c r="F17" s="8">
+        <v>4.16073</v>
+      </c>
+      <c r="G17" s="8">
+        <v>3.9509099999999999</v>
+      </c>
+      <c r="H17" s="9">
+        <v>1.7260000000000001E-2</v>
+      </c>
+      <c r="I17" s="18">
+        <v>1.2404900000000001</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1.26959</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1.25203</v>
+      </c>
+      <c r="L17" s="22">
+        <v>7.3699999999999998E-3</v>
+      </c>
+      <c r="M17" s="7">
+        <v>4.3073300000000003</v>
+      </c>
+      <c r="N17" s="8">
+        <v>4.3084899999999999</v>
+      </c>
+      <c r="O17" s="8">
+        <v>4.3078599999999998</v>
+      </c>
+      <c r="P17" s="9">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>7.0112699999999997</v>
+      </c>
+      <c r="R17" s="8">
+        <v>7.0221200000000001</v>
+      </c>
+      <c r="S17" s="8">
+        <v>7.0131800000000002</v>
+      </c>
+      <c r="T17" s="9">
+        <v>6.6E-4</v>
+      </c>
     </row>
     <row r="18" spans="2:20">
       <c r="B18" s="40"/>
@@ -1498,22 +1946,54 @@
       <c r="D18" s="14">
         <v>100</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="9"/>
+      <c r="E18" s="7">
+        <v>4.2616300000000003</v>
+      </c>
+      <c r="F18" s="8">
+        <v>4.5187499999999998</v>
+      </c>
+      <c r="G18" s="8">
+        <v>4.2636500000000002</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1.5939999999999999E-2</v>
+      </c>
+      <c r="I18" s="18">
+        <v>1.42075</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1.47797</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1.4214100000000001</v>
+      </c>
+      <c r="L18" s="22">
+        <v>3.7299999999999998E-3</v>
+      </c>
+      <c r="M18" s="7">
+        <v>4.3069100000000002</v>
+      </c>
+      <c r="N18" s="8">
+        <v>4.31114</v>
+      </c>
+      <c r="O18" s="8">
+        <v>4.3069899999999999</v>
+      </c>
+      <c r="P18" s="9">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="Q18" s="18">
+        <v>7.0069800000000004</v>
+      </c>
+      <c r="R18" s="8">
+        <v>7.0698100000000004</v>
+      </c>
+      <c r="S18" s="8">
+        <v>7.0098799999999999</v>
+      </c>
+      <c r="T18" s="9">
+        <v>4.9699999999999996E-3</v>
+      </c>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickBot="1">
       <c r="B19" s="41"/>
@@ -1521,22 +2001,54 @@
       <c r="D19" s="15">
         <v>250</v>
       </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="12"/>
+      <c r="E19" s="10">
+        <v>3.7141000000000002</v>
+      </c>
+      <c r="F19" s="11">
+        <v>3.7358099999999999</v>
+      </c>
+      <c r="G19" s="11">
+        <v>3.7159399999999998</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1.49E-3</v>
+      </c>
+      <c r="I19" s="19">
+        <v>1.1674500000000001</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1.2197100000000001</v>
+      </c>
+      <c r="K19" s="11">
+        <v>1.16771</v>
+      </c>
+      <c r="L19" s="23">
+        <v>2.97E-3</v>
+      </c>
+      <c r="M19" s="10">
+        <v>4.3093700000000004</v>
+      </c>
+      <c r="N19" s="11">
+        <v>4.3568300000000004</v>
+      </c>
+      <c r="O19" s="11">
+        <v>4.3096100000000002</v>
+      </c>
+      <c r="P19" s="12">
+        <v>2.6800000000000001E-3</v>
+      </c>
+      <c r="Q19" s="19">
+        <v>6.9993499999999997</v>
+      </c>
+      <c r="R19" s="11">
+        <v>6.9993600000000002</v>
+      </c>
+      <c r="S19" s="11">
+        <v>6.9993600000000002</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:20">
       <c r="B20" s="40"/>
@@ -1544,22 +2056,54 @@
       <c r="D20" s="13">
         <v>20</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="17"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="6"/>
+      <c r="E20" s="4">
+        <v>14.16479</v>
+      </c>
+      <c r="F20" s="5">
+        <v>15.118980000000001</v>
+      </c>
+      <c r="G20" s="5">
+        <v>14.842510000000001</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.24912999999999999</v>
+      </c>
+      <c r="I20" s="17">
+        <v>3.7420599999999999</v>
+      </c>
+      <c r="J20" s="5">
+        <v>3.94068</v>
+      </c>
+      <c r="K20" s="5">
+        <v>3.8706900000000002</v>
+      </c>
+      <c r="L20" s="21">
+        <v>8.3349999999999994E-2</v>
+      </c>
+      <c r="M20" s="4">
+        <v>12.44783</v>
+      </c>
+      <c r="N20" s="5">
+        <v>13.16114</v>
+      </c>
+      <c r="O20" s="5">
+        <v>12.82516</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0.26674999999999999</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>8.8998600000000003</v>
+      </c>
+      <c r="R20" s="5">
+        <v>9.5131300000000003</v>
+      </c>
+      <c r="S20" s="5">
+        <v>9.0167199999999994</v>
+      </c>
+      <c r="T20" s="6">
+        <v>0.16622999999999999</v>
+      </c>
     </row>
     <row r="21" spans="2:20">
       <c r="B21" s="40"/>
@@ -1567,22 +2111,54 @@
       <c r="D21" s="14">
         <v>50</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="9"/>
+      <c r="E21" s="7">
+        <v>10.48251</v>
+      </c>
+      <c r="F21" s="8">
+        <v>10.48465</v>
+      </c>
+      <c r="G21" s="8">
+        <v>10.48418</v>
+      </c>
+      <c r="H21" s="9">
+        <v>6.2E-4</v>
+      </c>
+      <c r="I21" s="18">
+        <v>3.1495700000000002</v>
+      </c>
+      <c r="J21" s="8">
+        <v>3.3532299999999999</v>
+      </c>
+      <c r="K21" s="8">
+        <v>3.1540400000000002</v>
+      </c>
+      <c r="L21" s="22">
+        <v>2.8459999999999999E-2</v>
+      </c>
+      <c r="M21" s="7">
+        <v>9.5051000000000005</v>
+      </c>
+      <c r="N21" s="8">
+        <v>9.51051</v>
+      </c>
+      <c r="O21" s="8">
+        <v>9.5062599999999993</v>
+      </c>
+      <c r="P21" s="9">
+        <v>1.15E-3</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>9.1643299999999996</v>
+      </c>
+      <c r="R21" s="8">
+        <v>9.2851900000000001</v>
+      </c>
+      <c r="S21" s="8">
+        <v>9.23095</v>
+      </c>
+      <c r="T21" s="9">
+        <v>2.554E-2</v>
+      </c>
     </row>
     <row r="22" spans="2:20">
       <c r="B22" s="40"/>
@@ -1592,22 +2168,54 @@
       <c r="D22" s="14">
         <v>100</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="9"/>
+      <c r="E22" s="7">
+        <v>9.6260999999999992</v>
+      </c>
+      <c r="F22" s="8">
+        <v>9.6323799999999995</v>
+      </c>
+      <c r="G22" s="8">
+        <v>9.6282399999999999</v>
+      </c>
+      <c r="H22" s="9">
+        <v>1.99E-3</v>
+      </c>
+      <c r="I22" s="18">
+        <v>2.3039499999999999</v>
+      </c>
+      <c r="J22" s="8">
+        <v>2.3521100000000001</v>
+      </c>
+      <c r="K22" s="8">
+        <v>2.3479899999999998</v>
+      </c>
+      <c r="L22" s="22">
+        <v>6.4599999999999996E-3</v>
+      </c>
+      <c r="M22" s="7">
+        <v>8.2632399999999997</v>
+      </c>
+      <c r="N22" s="8">
+        <v>10.09168</v>
+      </c>
+      <c r="O22" s="8">
+        <v>8.4131999999999998</v>
+      </c>
+      <c r="P22" s="9">
+        <v>0.24035000000000001</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>8.3141499999999997</v>
+      </c>
+      <c r="R22" s="8">
+        <v>8.3453400000000002</v>
+      </c>
+      <c r="S22" s="8">
+        <v>8.33582</v>
+      </c>
+      <c r="T22" s="9">
+        <v>9.7199999999999995E-3</v>
+      </c>
     </row>
     <row r="23" spans="2:20" ht="15.75" thickBot="1">
       <c r="B23" s="40"/>
@@ -1615,22 +2223,54 @@
       <c r="D23" s="29">
         <v>250</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="25"/>
-      <c r="O23" s="25"/>
-      <c r="P23" s="26"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="25"/>
-      <c r="S23" s="25"/>
-      <c r="T23" s="26"/>
+      <c r="E23" s="24">
+        <v>7.8182700000000001</v>
+      </c>
+      <c r="F23" s="25">
+        <v>8.5290599999999994</v>
+      </c>
+      <c r="G23" s="25">
+        <v>7.8335699999999999</v>
+      </c>
+      <c r="H23" s="26">
+        <v>9.9409999999999998E-2</v>
+      </c>
+      <c r="I23" s="27">
+        <v>2.0446800000000001</v>
+      </c>
+      <c r="J23" s="25">
+        <v>2.0446800000000001</v>
+      </c>
+      <c r="K23" s="25">
+        <v>2.0446800000000001</v>
+      </c>
+      <c r="L23" s="28">
+        <v>0</v>
+      </c>
+      <c r="M23" s="24">
+        <v>6.1516000000000002</v>
+      </c>
+      <c r="N23" s="25">
+        <v>6.1516200000000003</v>
+      </c>
+      <c r="O23" s="25">
+        <v>6.1516099999999998</v>
+      </c>
+      <c r="P23" s="26">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="Q23" s="27">
+        <v>7.7038900000000003</v>
+      </c>
+      <c r="R23" s="25">
+        <v>8.3019099999999995</v>
+      </c>
+      <c r="S23" s="25">
+        <v>7.7158499999999997</v>
+      </c>
+      <c r="T23" s="26">
+        <v>8.3720000000000003E-2</v>
+      </c>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="40"/>
@@ -1638,22 +2278,54 @@
       <c r="D24" s="13">
         <v>20</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="6"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="6"/>
+      <c r="E24" s="4">
+        <v>11.27291</v>
+      </c>
+      <c r="F24" s="5">
+        <v>12.27258</v>
+      </c>
+      <c r="G24" s="5">
+        <v>11.913740000000001</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0.20723</v>
+      </c>
+      <c r="I24" s="17">
+        <v>3.1882799999999998</v>
+      </c>
+      <c r="J24" s="5">
+        <v>3.5406900000000001</v>
+      </c>
+      <c r="K24" s="5">
+        <v>3.39628</v>
+      </c>
+      <c r="L24" s="21">
+        <v>6.7489999999999994E-2</v>
+      </c>
+      <c r="M24" s="4">
+        <v>11.854290000000001</v>
+      </c>
+      <c r="N24" s="5">
+        <v>12.87613</v>
+      </c>
+      <c r="O24" s="5">
+        <v>12.3855</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0.22832</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>9.3361000000000001</v>
+      </c>
+      <c r="R24" s="5">
+        <v>9.8754600000000003</v>
+      </c>
+      <c r="S24" s="5">
+        <v>9.6119699999999995</v>
+      </c>
+      <c r="T24" s="6">
+        <v>0.15079999999999999</v>
+      </c>
     </row>
     <row r="25" spans="2:20">
       <c r="B25" s="40"/>
@@ -1661,22 +2333,54 @@
       <c r="D25" s="14">
         <v>50</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="9"/>
+      <c r="E25" s="7">
+        <v>8.16479</v>
+      </c>
+      <c r="F25" s="8">
+        <v>8.3330400000000004</v>
+      </c>
+      <c r="G25" s="8">
+        <v>8.3261599999999998</v>
+      </c>
+      <c r="H25" s="9">
+        <v>2.9319999999999999E-2</v>
+      </c>
+      <c r="I25" s="18">
+        <v>2.8186800000000001</v>
+      </c>
+      <c r="J25" s="8">
+        <v>2.9344199999999998</v>
+      </c>
+      <c r="K25" s="8">
+        <v>2.8668399999999998</v>
+      </c>
+      <c r="L25" s="22">
+        <v>2.0060000000000001E-2</v>
+      </c>
+      <c r="M25" s="7">
+        <v>8.9730600000000003</v>
+      </c>
+      <c r="N25" s="8">
+        <v>9.0459800000000001</v>
+      </c>
+      <c r="O25" s="8">
+        <v>9.0165299999999995</v>
+      </c>
+      <c r="P25" s="9">
+        <v>2.792E-2</v>
+      </c>
+      <c r="Q25" s="18">
+        <v>7.8670799999999996</v>
+      </c>
+      <c r="R25" s="8">
+        <v>8.1242800000000006</v>
+      </c>
+      <c r="S25" s="8">
+        <v>7.8955200000000003</v>
+      </c>
+      <c r="T25" s="9">
+        <v>3.5740000000000001E-2</v>
+      </c>
     </row>
     <row r="26" spans="2:20">
       <c r="B26" s="40"/>
@@ -1686,22 +2390,54 @@
       <c r="D26" s="14">
         <v>100</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="9"/>
+      <c r="E26" s="7">
+        <v>6.4257600000000004</v>
+      </c>
+      <c r="F26" s="8">
+        <v>6.4281600000000001</v>
+      </c>
+      <c r="G26" s="8">
+        <v>6.4267200000000004</v>
+      </c>
+      <c r="H26" s="9">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I26" s="18">
+        <v>2.1204299999999998</v>
+      </c>
+      <c r="J26" s="8">
+        <v>2.2349000000000001</v>
+      </c>
+      <c r="K26" s="8">
+        <v>2.1841400000000002</v>
+      </c>
+      <c r="L26" s="22">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="M26" s="7">
+        <v>6.9809400000000004</v>
+      </c>
+      <c r="N26" s="8">
+        <v>7.1061500000000004</v>
+      </c>
+      <c r="O26" s="8">
+        <v>6.9833600000000002</v>
+      </c>
+      <c r="P26" s="9">
+        <v>1.4670000000000001E-2</v>
+      </c>
+      <c r="Q26" s="18">
+        <v>7.3479000000000001</v>
+      </c>
+      <c r="R26" s="8">
+        <v>7.3535500000000003</v>
+      </c>
+      <c r="S26" s="8">
+        <v>7.3508599999999999</v>
+      </c>
+      <c r="T26" s="9">
+        <v>9.6000000000000002E-4</v>
+      </c>
     </row>
     <row r="27" spans="2:20" ht="15.75" thickBot="1">
       <c r="B27" s="40">
@@ -1711,22 +2447,54 @@
       <c r="D27" s="29">
         <v>250</v>
       </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="25"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="26"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="25"/>
-      <c r="S27" s="25"/>
-      <c r="T27" s="26"/>
+      <c r="E27" s="24">
+        <v>5.5345700000000004</v>
+      </c>
+      <c r="F27" s="25">
+        <v>5.5364399999999998</v>
+      </c>
+      <c r="G27" s="25">
+        <v>5.5364199999999997</v>
+      </c>
+      <c r="H27" s="26">
+        <v>1.9000000000000001E-4</v>
+      </c>
+      <c r="I27" s="27">
+        <v>1.5249200000000001</v>
+      </c>
+      <c r="J27" s="25">
+        <v>1.5289600000000001</v>
+      </c>
+      <c r="K27" s="25">
+        <v>1.52599</v>
+      </c>
+      <c r="L27" s="28">
+        <v>9.7999999999999997E-4</v>
+      </c>
+      <c r="M27" s="24">
+        <v>5.9854500000000002</v>
+      </c>
+      <c r="N27" s="25">
+        <v>6.8130499999999996</v>
+      </c>
+      <c r="O27" s="25">
+        <v>6.05206</v>
+      </c>
+      <c r="P27" s="26">
+        <v>8.9389999999999997E-2</v>
+      </c>
+      <c r="Q27" s="27">
+        <v>7.3736899999999999</v>
+      </c>
+      <c r="R27" s="25">
+        <v>7.3783700000000003</v>
+      </c>
+      <c r="S27" s="25">
+        <v>7.3755699999999997</v>
+      </c>
+      <c r="T27" s="26">
+        <v>1.0399999999999999E-3</v>
+      </c>
     </row>
     <row r="28" spans="2:20">
       <c r="B28" s="40"/>
@@ -1734,22 +2502,54 @@
       <c r="D28" s="13">
         <v>20</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="6"/>
+      <c r="E28" s="4">
+        <v>9.4624400000000009</v>
+      </c>
+      <c r="F28" s="5">
+        <v>11.31256</v>
+      </c>
+      <c r="G28" s="5">
+        <v>10.46608</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.37935999999999998</v>
+      </c>
+      <c r="I28" s="17">
+        <v>2.8256299999999999</v>
+      </c>
+      <c r="J28" s="5">
+        <v>3.5810399999999998</v>
+      </c>
+      <c r="K28" s="5">
+        <v>3.2328700000000001</v>
+      </c>
+      <c r="L28" s="21">
+        <v>0.14346999999999999</v>
+      </c>
+      <c r="M28" s="4">
+        <v>8.3663500000000006</v>
+      </c>
+      <c r="N28" s="5">
+        <v>11.413880000000001</v>
+      </c>
+      <c r="O28" s="5">
+        <v>9.9222099999999998</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0.52003999999999995</v>
+      </c>
+      <c r="Q28" s="17">
+        <v>8.8729200000000006</v>
+      </c>
+      <c r="R28" s="5">
+        <v>9.3040400000000005</v>
+      </c>
+      <c r="S28" s="5">
+        <v>9.1040200000000002</v>
+      </c>
+      <c r="T28" s="6">
+        <v>9.6909999999999996E-2</v>
+      </c>
     </row>
     <row r="29" spans="2:20">
       <c r="B29" s="40"/>
@@ -1757,22 +2557,54 @@
       <c r="D29" s="14">
         <v>50</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="18"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="9"/>
+      <c r="E29" s="7">
+        <v>7.1971499999999997</v>
+      </c>
+      <c r="F29" s="8">
+        <v>7.4829999999999997</v>
+      </c>
+      <c r="G29" s="8">
+        <v>7.3814500000000001</v>
+      </c>
+      <c r="H29" s="9">
+        <v>4.4769999999999997E-2</v>
+      </c>
+      <c r="I29" s="18">
+        <v>2.31975</v>
+      </c>
+      <c r="J29" s="8">
+        <v>2.6159599999999998</v>
+      </c>
+      <c r="K29" s="8">
+        <v>2.3641200000000002</v>
+      </c>
+      <c r="L29" s="22">
+        <v>2.9839999999999998E-2</v>
+      </c>
+      <c r="M29" s="7">
+        <v>9.1546000000000003</v>
+      </c>
+      <c r="N29" s="8">
+        <v>9.1866000000000003</v>
+      </c>
+      <c r="O29" s="8">
+        <v>9.1828599999999998</v>
+      </c>
+      <c r="P29" s="9">
+        <v>4.2700000000000004E-3</v>
+      </c>
+      <c r="Q29" s="18">
+        <v>7.7617500000000001</v>
+      </c>
+      <c r="R29" s="8">
+        <v>7.8848700000000003</v>
+      </c>
+      <c r="S29" s="8">
+        <v>7.7747900000000003</v>
+      </c>
+      <c r="T29" s="9">
+        <v>1.47E-2</v>
+      </c>
     </row>
     <row r="30" spans="2:20">
       <c r="B30" s="40"/>
@@ -1782,22 +2614,54 @@
       <c r="D30" s="14">
         <v>100</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="18"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="9"/>
+      <c r="E30" s="7">
+        <v>5.87819</v>
+      </c>
+      <c r="F30" s="8">
+        <v>6.2587000000000002</v>
+      </c>
+      <c r="G30" s="8">
+        <v>6.1649099999999999</v>
+      </c>
+      <c r="H30" s="9">
+        <v>8.856E-2</v>
+      </c>
+      <c r="I30" s="18">
+        <v>2.0583</v>
+      </c>
+      <c r="J30" s="8">
+        <v>2.06609</v>
+      </c>
+      <c r="K30" s="8">
+        <v>2.0588199999999999</v>
+      </c>
+      <c r="L30" s="22">
+        <v>1.17E-3</v>
+      </c>
+      <c r="M30" s="7">
+        <v>5.1202100000000002</v>
+      </c>
+      <c r="N30" s="8">
+        <v>5.1296400000000002</v>
+      </c>
+      <c r="O30" s="8">
+        <v>5.1295599999999997</v>
+      </c>
+      <c r="P30" s="9">
+        <v>6.7000000000000002E-4</v>
+      </c>
+      <c r="Q30" s="18">
+        <v>7.2952399999999997</v>
+      </c>
+      <c r="R30" s="8">
+        <v>7.3734500000000001</v>
+      </c>
+      <c r="S30" s="8">
+        <v>7.3128299999999999</v>
+      </c>
+      <c r="T30" s="9">
+        <v>1.0449999999999999E-2</v>
+      </c>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1">
       <c r="B31" s="40"/>
@@ -1805,22 +2669,54 @@
       <c r="D31" s="29">
         <v>250</v>
       </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="24"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="26"/>
-      <c r="Q31" s="27"/>
-      <c r="R31" s="25"/>
-      <c r="S31" s="25"/>
-      <c r="T31" s="26"/>
+      <c r="E31" s="24">
+        <v>5.7364100000000002</v>
+      </c>
+      <c r="F31" s="25">
+        <v>5.7387300000000003</v>
+      </c>
+      <c r="G31" s="25">
+        <v>5.73848</v>
+      </c>
+      <c r="H31" s="26">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="I31" s="27">
+        <v>1.70709</v>
+      </c>
+      <c r="J31" s="25">
+        <v>1.7083600000000001</v>
+      </c>
+      <c r="K31" s="25">
+        <v>1.7079599999999999</v>
+      </c>
+      <c r="L31" s="28">
+        <v>5.9000000000000003E-4</v>
+      </c>
+      <c r="M31" s="24">
+        <v>5.1379000000000001</v>
+      </c>
+      <c r="N31" s="25">
+        <v>5.1675399999999998</v>
+      </c>
+      <c r="O31" s="25">
+        <v>5.1658799999999996</v>
+      </c>
+      <c r="P31" s="26">
+        <v>2.5899999999999999E-3</v>
+      </c>
+      <c r="Q31" s="27">
+        <v>7.0989800000000001</v>
+      </c>
+      <c r="R31" s="25">
+        <v>7.1004800000000001</v>
+      </c>
+      <c r="S31" s="25">
+        <v>7.0994200000000003</v>
+      </c>
+      <c r="T31" s="26">
+        <v>5.6999999999999998E-4</v>
+      </c>
     </row>
     <row r="32" spans="2:20">
       <c r="B32" s="40"/>
@@ -1828,22 +2724,54 @@
       <c r="D32" s="13">
         <v>20</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="6"/>
+      <c r="E32" s="4">
+        <v>7.7546799999999996</v>
+      </c>
+      <c r="F32" s="5">
+        <v>10.843159999999999</v>
+      </c>
+      <c r="G32" s="5">
+        <v>9.5026700000000002</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0.61887999999999999</v>
+      </c>
+      <c r="I32" s="17">
+        <v>2.5909300000000002</v>
+      </c>
+      <c r="J32" s="5">
+        <v>3.5800800000000002</v>
+      </c>
+      <c r="K32" s="5">
+        <v>3.0800299999999998</v>
+      </c>
+      <c r="L32" s="21">
+        <v>0.19383</v>
+      </c>
+      <c r="M32" s="4">
+        <v>8.1118500000000004</v>
+      </c>
+      <c r="N32" s="5">
+        <v>11.82802</v>
+      </c>
+      <c r="O32" s="5">
+        <v>10.042070000000001</v>
+      </c>
+      <c r="P32" s="6">
+        <v>0.80356000000000005</v>
+      </c>
+      <c r="Q32" s="17">
+        <v>7.9769199999999998</v>
+      </c>
+      <c r="R32" s="5">
+        <v>8.7054299999999998</v>
+      </c>
+      <c r="S32" s="5">
+        <v>8.3784799999999997</v>
+      </c>
+      <c r="T32" s="6">
+        <v>0.14526</v>
+      </c>
     </row>
     <row r="33" spans="2:20">
       <c r="B33" s="40"/>
@@ -1851,22 +2779,54 @@
       <c r="D33" s="14">
         <v>50</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="9"/>
+      <c r="E33" s="7">
+        <v>5.9109499999999997</v>
+      </c>
+      <c r="F33" s="8">
+        <v>6.2038900000000003</v>
+      </c>
+      <c r="G33" s="8">
+        <v>6.0258200000000004</v>
+      </c>
+      <c r="H33" s="9">
+        <v>3.619E-2</v>
+      </c>
+      <c r="I33" s="18">
+        <v>1.69913</v>
+      </c>
+      <c r="J33" s="8">
+        <v>1.74719</v>
+      </c>
+      <c r="K33" s="8">
+        <v>1.72322</v>
+      </c>
+      <c r="L33" s="22">
+        <v>8.5500000000000003E-3</v>
+      </c>
+      <c r="M33" s="7">
+        <v>5.24573</v>
+      </c>
+      <c r="N33" s="8">
+        <v>5.6530699999999996</v>
+      </c>
+      <c r="O33" s="8">
+        <v>5.3084100000000003</v>
+      </c>
+      <c r="P33" s="9">
+        <v>6.0819999999999999E-2</v>
+      </c>
+      <c r="Q33" s="18">
+        <v>7.4146700000000001</v>
+      </c>
+      <c r="R33" s="8">
+        <v>7.4894400000000001</v>
+      </c>
+      <c r="S33" s="8">
+        <v>7.4648199999999996</v>
+      </c>
+      <c r="T33" s="9">
+        <v>1.244E-2</v>
+      </c>
     </row>
     <row r="34" spans="2:20">
       <c r="B34" s="40"/>
@@ -1876,22 +2836,54 @@
       <c r="D34" s="14">
         <v>100</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="T34" s="9"/>
+      <c r="E34" s="7">
+        <v>5.1412500000000003</v>
+      </c>
+      <c r="F34" s="8">
+        <v>5.2931400000000002</v>
+      </c>
+      <c r="G34" s="8">
+        <v>5.1932999999999998</v>
+      </c>
+      <c r="H34" s="9">
+        <v>1.7809999999999999E-2</v>
+      </c>
+      <c r="I34" s="18">
+        <v>1.8016399999999999</v>
+      </c>
+      <c r="J34" s="8">
+        <v>1.8089999999999999</v>
+      </c>
+      <c r="K34" s="8">
+        <v>1.80437</v>
+      </c>
+      <c r="L34" s="22">
+        <v>1.72E-3</v>
+      </c>
+      <c r="M34" s="7">
+        <v>5.2156500000000001</v>
+      </c>
+      <c r="N34" s="8">
+        <v>5.2164000000000001</v>
+      </c>
+      <c r="O34" s="8">
+        <v>5.2159500000000003</v>
+      </c>
+      <c r="P34" s="9">
+        <v>3.1E-4</v>
+      </c>
+      <c r="Q34" s="18">
+        <v>7.3427699999999998</v>
+      </c>
+      <c r="R34" s="8">
+        <v>7.3510999999999997</v>
+      </c>
+      <c r="S34" s="8">
+        <v>7.3476600000000003</v>
+      </c>
+      <c r="T34" s="9">
+        <v>1.65E-3</v>
+      </c>
     </row>
     <row r="35" spans="2:20" ht="15.75" thickBot="1">
       <c r="B35" s="41"/>
@@ -1899,22 +2891,54 @@
       <c r="D35" s="15">
         <v>250</v>
       </c>
-      <c r="E35" s="10"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="12"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="12"/>
+      <c r="E35" s="10">
+        <v>4.31182</v>
+      </c>
+      <c r="F35" s="11">
+        <v>4.3266200000000001</v>
+      </c>
+      <c r="G35" s="11">
+        <v>4.3261799999999999</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1.5900000000000001E-3</v>
+      </c>
+      <c r="I35" s="19">
+        <v>1.5556700000000001</v>
+      </c>
+      <c r="J35" s="11">
+        <v>1.5609200000000001</v>
+      </c>
+      <c r="K35" s="11">
+        <v>1.55951</v>
+      </c>
+      <c r="L35" s="23">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="M35" s="10">
+        <v>4.7808099999999998</v>
+      </c>
+      <c r="N35" s="11">
+        <v>4.7817299999999996</v>
+      </c>
+      <c r="O35" s="11">
+        <v>4.7809799999999996</v>
+      </c>
+      <c r="P35" s="12">
+        <v>3.4000000000000002E-4</v>
+      </c>
+      <c r="Q35" s="19">
+        <v>7.1435700000000004</v>
+      </c>
+      <c r="R35" s="11">
+        <v>7.1440799999999998</v>
+      </c>
+      <c r="S35" s="11">
+        <v>7.1437200000000001</v>
+      </c>
+      <c r="T35" s="12">
+        <v>2.3000000000000001E-4</v>
+      </c>
     </row>
     <row r="37" spans="2:20" ht="15.75" thickBot="1"/>
     <row r="38" spans="2:20" ht="15.75" thickBot="1">
@@ -2875,8 +3899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:T75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2991,52 +4015,52 @@
         <v>20</v>
       </c>
       <c r="E4" s="4">
-        <v>5.3469600000000002</v>
+        <v>6.2524100000000002</v>
       </c>
       <c r="F4" s="5">
-        <v>6.0959300000000001</v>
+        <v>6.8687899999999997</v>
       </c>
       <c r="G4" s="5">
-        <v>6.0384399999999996</v>
+        <v>6.5760100000000001</v>
       </c>
       <c r="H4" s="6">
-        <v>9.8979999999999999E-2</v>
+        <v>0.15429000000000001</v>
       </c>
       <c r="I4" s="17">
-        <v>1.77542</v>
+        <v>2.3530700000000002</v>
       </c>
       <c r="J4" s="5">
-        <v>1.9542600000000001</v>
+        <v>2.63612</v>
       </c>
       <c r="K4" s="5">
-        <v>1.83097</v>
+        <v>2.4989599999999998</v>
       </c>
       <c r="L4" s="21">
-        <v>3.2590000000000001E-2</v>
+        <v>9.9140000000000006E-2</v>
       </c>
       <c r="M4" s="4">
-        <v>4.9880699999999996</v>
+        <v>4.8688000000000002</v>
       </c>
       <c r="N4" s="5">
-        <v>5.3151999999999999</v>
+        <v>4.86883</v>
       </c>
       <c r="O4" s="5">
-        <v>5.1927399999999997</v>
+        <v>4.86883</v>
       </c>
       <c r="P4" s="6">
-        <v>0.10763</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q4" s="17">
-        <v>7.62723</v>
+        <v>7.4522899999999996</v>
       </c>
       <c r="R4" s="5">
-        <v>7.7290000000000001</v>
+        <v>7.7223100000000002</v>
       </c>
       <c r="S4" s="5">
-        <v>7.6502499999999998</v>
+        <v>7.6476800000000003</v>
       </c>
       <c r="T4" s="6">
-        <v>2.283E-2</v>
+        <v>5.3249999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="2:20">
@@ -3046,52 +4070,52 @@
         <v>50</v>
       </c>
       <c r="E5" s="7">
-        <v>4.4558299999999997</v>
+        <v>5.4174800000000003</v>
       </c>
       <c r="F5" s="8">
-        <v>5.0983900000000002</v>
+        <v>5.4807199999999998</v>
       </c>
       <c r="G5" s="8">
-        <v>4.4987399999999997</v>
+        <v>5.4392500000000004</v>
       </c>
       <c r="H5" s="9">
-        <v>0.13300000000000001</v>
+        <v>1.694E-2</v>
       </c>
       <c r="I5" s="18">
-        <v>1.7860199999999999</v>
+        <v>1.52651</v>
       </c>
       <c r="J5" s="8">
-        <v>1.8094399999999999</v>
+        <v>1.93228</v>
       </c>
       <c r="K5" s="8">
-        <v>1.78901</v>
+        <v>1.58579</v>
       </c>
       <c r="L5" s="22">
-        <v>4.4400000000000004E-3</v>
+        <v>5.7950000000000002E-2</v>
       </c>
       <c r="M5" s="7">
-        <v>5.7182000000000004</v>
+        <v>5.7152599999999998</v>
       </c>
       <c r="N5" s="8">
-        <v>5.7187400000000004</v>
+        <v>5.7155500000000004</v>
       </c>
       <c r="O5" s="8">
-        <v>5.7187200000000002</v>
+        <v>5.7154699999999998</v>
       </c>
       <c r="P5" s="9">
-        <v>1.1E-4</v>
+        <v>3.0000000000000001E-5</v>
       </c>
       <c r="Q5" s="18">
-        <v>7.2088000000000001</v>
+        <v>7.41411</v>
       </c>
       <c r="R5" s="8">
-        <v>7.2938799999999997</v>
+        <v>7.4700300000000004</v>
       </c>
       <c r="S5" s="8">
-        <v>7.2119</v>
+        <v>7.4526500000000002</v>
       </c>
       <c r="T5" s="9">
-        <v>1.34E-2</v>
+        <v>1.306E-2</v>
       </c>
     </row>
     <row r="6" spans="2:20">
@@ -3103,52 +4127,52 @@
         <v>100</v>
       </c>
       <c r="E6" s="7">
-        <v>5.2099700000000002</v>
+        <v>4.8801899999999998</v>
       </c>
       <c r="F6" s="8">
-        <v>5.2261300000000004</v>
+        <v>4.8801899999999998</v>
       </c>
       <c r="G6" s="8">
-        <v>5.2257999999999996</v>
+        <v>4.8801899999999998</v>
       </c>
       <c r="H6" s="9">
-        <v>2.2599999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="I6" s="18">
-        <v>1.7373099999999999</v>
+        <v>1.55077</v>
       </c>
       <c r="J6" s="8">
-        <v>1.7649699999999999</v>
+        <v>1.5515399999999999</v>
       </c>
       <c r="K6" s="8">
-        <v>1.7502899999999999</v>
+        <v>1.5508200000000001</v>
       </c>
       <c r="L6" s="22">
-        <v>1.021E-2</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="M6" s="7">
-        <v>4.8492899999999999</v>
+        <v>4.3401300000000003</v>
       </c>
       <c r="N6" s="8">
-        <v>4.8492899999999999</v>
+        <v>4.3409199999999997</v>
       </c>
       <c r="O6" s="8">
-        <v>4.8492899999999999</v>
+        <v>4.3407499999999999</v>
       </c>
       <c r="P6" s="9">
-        <v>0</v>
+        <v>3.2000000000000003E-4</v>
       </c>
       <c r="Q6" s="18">
-        <v>7.1349600000000004</v>
+        <v>7.0938400000000001</v>
       </c>
       <c r="R6" s="8">
-        <v>7.1349600000000004</v>
+        <v>7.2479699999999996</v>
       </c>
       <c r="S6" s="8">
-        <v>7.1349600000000004</v>
+        <v>7.1264000000000003</v>
       </c>
       <c r="T6" s="9">
-        <v>0</v>
+        <v>1.9279999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="2:20" ht="15.75" thickBot="1">
@@ -3158,52 +4182,52 @@
         <v>250</v>
       </c>
       <c r="E7" s="24">
-        <v>4.8487999999999998</v>
+        <v>4.8395000000000001</v>
       </c>
       <c r="F7" s="25">
-        <v>4.8501599999999998</v>
+        <v>4.8430499999999999</v>
       </c>
       <c r="G7" s="25">
-        <v>4.84945</v>
+        <v>4.8429799999999998</v>
       </c>
       <c r="H7" s="26">
-        <v>6.8000000000000005E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="I7" s="27">
-        <v>1.3675200000000001</v>
+        <v>1.53481</v>
       </c>
       <c r="J7" s="25">
-        <v>1.3780699999999999</v>
+        <v>1.53481</v>
       </c>
       <c r="K7" s="25">
-        <v>1.3720000000000001</v>
+        <v>1.53481</v>
       </c>
       <c r="L7" s="28">
-        <v>3.4099999999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="M7" s="24">
-        <v>4.36205</v>
+        <v>4.5890199999999997</v>
       </c>
       <c r="N7" s="25">
-        <v>4.3633499999999996</v>
+        <v>5.2868300000000001</v>
       </c>
       <c r="O7" s="25">
-        <v>4.3621299999999996</v>
+        <v>4.6371900000000004</v>
       </c>
       <c r="P7" s="26">
-        <v>1.8000000000000001E-4</v>
+        <v>0.14849999999999999</v>
       </c>
       <c r="Q7" s="27">
-        <v>7.0467899999999997</v>
+        <v>7.3557300000000003</v>
       </c>
       <c r="R7" s="25">
-        <v>7.0467899999999997</v>
+        <v>7.35649</v>
       </c>
       <c r="S7" s="25">
-        <v>7.0467899999999997</v>
+        <v>7.3564699999999998</v>
       </c>
       <c r="T7" s="26">
-        <v>0</v>
+        <v>1.1E-4</v>
       </c>
     </row>
     <row r="8" spans="2:20">
@@ -3213,52 +4237,52 @@
         <v>20</v>
       </c>
       <c r="E8" s="4">
-        <v>5.4897499999999999</v>
+        <v>4.8394000000000004</v>
       </c>
       <c r="F8" s="5">
-        <v>6.3765400000000003</v>
+        <v>6.3507899999999999</v>
       </c>
       <c r="G8" s="5">
-        <v>5.7605599999999999</v>
+        <v>5.50319</v>
       </c>
       <c r="H8" s="6">
-        <v>0.16854</v>
+        <v>0.24257000000000001</v>
       </c>
       <c r="I8" s="17">
-        <v>1.81576</v>
+        <v>1.7087600000000001</v>
       </c>
       <c r="J8" s="5">
-        <v>2.0869200000000001</v>
+        <v>2.0344099999999998</v>
       </c>
       <c r="K8" s="5">
-        <v>1.8643799999999999</v>
+        <v>1.7347999999999999</v>
       </c>
       <c r="L8" s="21">
-        <v>5.7259999999999998E-2</v>
+        <v>4.3889999999999998E-2</v>
       </c>
       <c r="M8" s="4">
-        <v>4.3403099999999997</v>
+        <v>4.3484299999999996</v>
       </c>
       <c r="N8" s="5">
-        <v>5.3033999999999999</v>
+        <v>4.76898</v>
       </c>
       <c r="O8" s="5">
-        <v>4.50997</v>
+        <v>4.5388799999999998</v>
       </c>
       <c r="P8" s="6">
-        <v>0.19423000000000001</v>
+        <v>0.17635999999999999</v>
       </c>
       <c r="Q8" s="17">
-        <v>7.2232599999999998</v>
+        <v>7.3398300000000001</v>
       </c>
       <c r="R8" s="5">
-        <v>7.2979700000000003</v>
+        <v>7.6631900000000002</v>
       </c>
       <c r="S8" s="5">
-        <v>7.2588299999999997</v>
+        <v>7.4836299999999998</v>
       </c>
       <c r="T8" s="6">
-        <v>1.4290000000000001E-2</v>
+        <v>7.8119999999999995E-2</v>
       </c>
     </row>
     <row r="9" spans="2:20">
@@ -3268,52 +4292,52 @@
         <v>50</v>
       </c>
       <c r="E9" s="7">
-        <v>4.8494900000000003</v>
+        <v>4.04251</v>
       </c>
       <c r="F9" s="8">
-        <v>5.6893000000000002</v>
+        <v>4.0621900000000002</v>
       </c>
       <c r="G9" s="8">
-        <v>4.8673099999999998</v>
+        <v>4.0498200000000004</v>
       </c>
       <c r="H9" s="9">
-        <v>0.10717</v>
+        <v>3.4499999999999999E-3</v>
       </c>
       <c r="I9" s="18">
-        <v>1.6011599999999999</v>
+        <v>1.6721600000000001</v>
       </c>
       <c r="J9" s="8">
-        <v>1.6447799999999999</v>
+        <v>1.69259</v>
       </c>
       <c r="K9" s="8">
-        <v>1.6398299999999999</v>
+        <v>1.6778299999999999</v>
       </c>
       <c r="L9" s="22">
-        <v>3.9199999999999999E-3</v>
+        <v>7.9699999999999997E-3</v>
       </c>
       <c r="M9" s="7">
-        <v>4.3118100000000004</v>
+        <v>4.9040999999999997</v>
       </c>
       <c r="N9" s="8">
-        <v>4.3194400000000002</v>
+        <v>5.1459400000000004</v>
       </c>
       <c r="O9" s="8">
-        <v>4.3141100000000003</v>
+        <v>5.0134600000000002</v>
       </c>
       <c r="P9" s="9">
-        <v>9.8999999999999999E-4</v>
+        <v>7.3359999999999995E-2</v>
       </c>
       <c r="Q9" s="18">
-        <v>7.1109799999999996</v>
+        <v>7.0624799999999999</v>
       </c>
       <c r="R9" s="8">
-        <v>7.1169200000000004</v>
+        <v>7.0724299999999998</v>
       </c>
       <c r="S9" s="8">
-        <v>7.1167999999999996</v>
+        <v>7.0676800000000002</v>
       </c>
       <c r="T9" s="9">
-        <v>8.3000000000000001E-4</v>
+        <v>3.0200000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="2:20">
@@ -3325,52 +4349,52 @@
         <v>100</v>
       </c>
       <c r="E10" s="7">
-        <v>5.8129400000000002</v>
+        <v>4.8343100000000003</v>
       </c>
       <c r="F10" s="8">
-        <v>5.8166500000000001</v>
+        <v>5.0566800000000001</v>
       </c>
       <c r="G10" s="8">
-        <v>5.8144499999999999</v>
+        <v>4.8366400000000001</v>
       </c>
       <c r="H10" s="9">
-        <v>5.4000000000000001E-4</v>
+        <v>2.213E-2</v>
       </c>
       <c r="I10" s="18">
-        <v>1.58602</v>
+        <v>1.3935200000000001</v>
       </c>
       <c r="J10" s="8">
-        <v>1.6061000000000001</v>
+        <v>1.3935200000000001</v>
       </c>
       <c r="K10" s="8">
-        <v>1.5911</v>
+        <v>1.3935200000000001</v>
       </c>
       <c r="L10" s="22">
-        <v>7.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="M10" s="7">
-        <v>4.3299200000000004</v>
+        <v>4.31088</v>
       </c>
       <c r="N10" s="8">
-        <v>4.5723399999999996</v>
+        <v>4.3121400000000003</v>
       </c>
       <c r="O10" s="8">
-        <v>4.3330000000000002</v>
+        <v>4.3120099999999999</v>
       </c>
       <c r="P10" s="9">
-        <v>2.4910000000000002E-2</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="Q10" s="18">
-        <v>7.0818599999999998</v>
+        <v>7.1184099999999999</v>
       </c>
       <c r="R10" s="8">
-        <v>7.1231</v>
+        <v>7.6154099999999998</v>
       </c>
       <c r="S10" s="8">
-        <v>7.0865299999999998</v>
+        <v>7.1336300000000001</v>
       </c>
       <c r="T10" s="9">
-        <v>6.1999999999999998E-3</v>
+        <v>6.5420000000000006E-2</v>
       </c>
     </row>
     <row r="11" spans="2:20" ht="15.75" thickBot="1">
@@ -3382,49 +4406,49 @@
         <v>250</v>
       </c>
       <c r="E11" s="24">
-        <v>3.6785899999999998</v>
+        <v>4.0576600000000003</v>
       </c>
       <c r="F11" s="25">
-        <v>3.6785899999999998</v>
+        <v>4.7495200000000004</v>
       </c>
       <c r="G11" s="25">
-        <v>3.6785899999999998</v>
+        <v>4.0721100000000003</v>
       </c>
       <c r="H11" s="26">
-        <v>0</v>
+        <v>6.9540000000000005E-2</v>
       </c>
       <c r="I11" s="27">
-        <v>1.6431100000000001</v>
+        <v>1.5241499999999999</v>
       </c>
       <c r="J11" s="25">
-        <v>1.64453</v>
+        <v>1.5242599999999999</v>
       </c>
       <c r="K11" s="25">
-        <v>1.64388</v>
+        <v>1.5242100000000001</v>
       </c>
       <c r="L11" s="28">
-        <v>6.9999999999999999E-4</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="M11" s="24">
-        <v>4.3828399999999998</v>
+        <v>4.4191700000000003</v>
       </c>
       <c r="N11" s="25">
-        <v>4.42</v>
+        <v>4.41927</v>
       </c>
       <c r="O11" s="25">
-        <v>4.3900499999999996</v>
+        <v>4.4192499999999999</v>
       </c>
       <c r="P11" s="26">
-        <v>1.323E-2</v>
+        <v>4.0000000000000003E-5</v>
       </c>
       <c r="Q11" s="27">
-        <v>7.0509399999999998</v>
+        <v>7.0064200000000003</v>
       </c>
       <c r="R11" s="25">
-        <v>7.0509399999999998</v>
+        <v>7.0064200000000003</v>
       </c>
       <c r="S11" s="25">
-        <v>7.0509399999999998</v>
+        <v>7.0064200000000003</v>
       </c>
       <c r="T11" s="26">
         <v>0</v>
@@ -3437,52 +4461,52 @@
         <v>20</v>
       </c>
       <c r="E12" s="4">
-        <v>5.04528</v>
+        <v>5.3399299999999998</v>
       </c>
       <c r="F12" s="5">
-        <v>5.3475900000000003</v>
+        <v>5.6481700000000004</v>
       </c>
       <c r="G12" s="5">
-        <v>5.1490400000000003</v>
+        <v>5.55002</v>
       </c>
       <c r="H12" s="6">
-        <v>6.8239999999999995E-2</v>
+        <v>5.7119999999999997E-2</v>
       </c>
       <c r="I12" s="17">
-        <v>1.45977</v>
+        <v>1.5423</v>
       </c>
       <c r="J12" s="5">
-        <v>1.9830300000000001</v>
+        <v>1.6991799999999999</v>
       </c>
       <c r="K12" s="5">
-        <v>1.64947</v>
+        <v>1.64022</v>
       </c>
       <c r="L12" s="21">
-        <v>9.7059999999999994E-2</v>
+        <v>3.7449999999999997E-2</v>
       </c>
       <c r="M12" s="4">
-        <v>4.8218399999999999</v>
+        <v>4.5678200000000002</v>
       </c>
       <c r="N12" s="5">
-        <v>5.3771000000000004</v>
+        <v>5.3767800000000001</v>
       </c>
       <c r="O12" s="5">
-        <v>5.0471300000000001</v>
+        <v>4.6834600000000002</v>
       </c>
       <c r="P12" s="6">
-        <v>0.13400000000000001</v>
+        <v>0.13028999999999999</v>
       </c>
       <c r="Q12" s="17">
-        <v>7.1345099999999997</v>
+        <v>7.29061</v>
       </c>
       <c r="R12" s="5">
-        <v>7.2616100000000001</v>
+        <v>7.6695399999999996</v>
       </c>
       <c r="S12" s="5">
-        <v>7.2085699999999999</v>
+        <v>7.4856299999999996</v>
       </c>
       <c r="T12" s="6">
-        <v>2.5739999999999999E-2</v>
+        <v>9.5530000000000004E-2</v>
       </c>
     </row>
     <row r="13" spans="2:20">
@@ -3492,52 +4516,52 @@
         <v>50</v>
       </c>
       <c r="E13" s="7">
-        <v>4.4726299999999997</v>
+        <v>4.1098600000000003</v>
       </c>
       <c r="F13" s="8">
-        <v>4.4981400000000002</v>
+        <v>4.2222400000000002</v>
       </c>
       <c r="G13" s="8">
-        <v>4.4919799999999999</v>
+        <v>4.1809099999999999</v>
       </c>
       <c r="H13" s="9">
-        <v>5.0499999999999998E-3</v>
+        <v>2.613E-2</v>
       </c>
       <c r="I13" s="18">
-        <v>1.21495</v>
+        <v>1.4998899999999999</v>
       </c>
       <c r="J13" s="8">
-        <v>1.2660899999999999</v>
+        <v>1.8000499999999999</v>
       </c>
       <c r="K13" s="8">
-        <v>1.2537400000000001</v>
+        <v>1.50166</v>
       </c>
       <c r="L13" s="22">
-        <v>6.94E-3</v>
+        <v>2.121E-2</v>
       </c>
       <c r="M13" s="7">
-        <v>4.3579400000000001</v>
+        <v>4.3820600000000001</v>
       </c>
       <c r="N13" s="8">
-        <v>4.36029</v>
+        <v>4.3820600000000001</v>
       </c>
       <c r="O13" s="8">
-        <v>4.3589099999999998</v>
+        <v>4.3820600000000001</v>
       </c>
       <c r="P13" s="9">
-        <v>9.6000000000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="18">
-        <v>7.0756399999999999</v>
+        <v>7.0463300000000002</v>
       </c>
       <c r="R13" s="8">
-        <v>7.0930200000000001</v>
+        <v>7.13992</v>
       </c>
       <c r="S13" s="8">
-        <v>7.0821199999999997</v>
+        <v>7.04758</v>
       </c>
       <c r="T13" s="9">
-        <v>4.3800000000000002E-3</v>
+        <v>7.2399999999999999E-3</v>
       </c>
     </row>
     <row r="14" spans="2:20">
@@ -3549,52 +4573,52 @@
         <v>100</v>
       </c>
       <c r="E14" s="7">
-        <v>3.9960599999999999</v>
+        <v>5.3002700000000003</v>
       </c>
       <c r="F14" s="8">
-        <v>4.2361000000000004</v>
+        <v>5.3269799999999998</v>
       </c>
       <c r="G14" s="8">
-        <v>3.9976500000000001</v>
+        <v>5.3027300000000004</v>
       </c>
       <c r="H14" s="9">
-        <v>1.7059999999999999E-2</v>
+        <v>2.2000000000000001E-3</v>
       </c>
       <c r="I14" s="18">
-        <v>1.3939999999999999</v>
+        <v>1.32304</v>
       </c>
       <c r="J14" s="8">
-        <v>1.39608</v>
+        <v>1.32304</v>
       </c>
       <c r="K14" s="8">
-        <v>1.3952500000000001</v>
+        <v>1.32304</v>
       </c>
       <c r="L14" s="22">
-        <v>5.0000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="M14" s="7">
-        <v>4.3122499999999997</v>
+        <v>4.31839</v>
       </c>
       <c r="N14" s="8">
-        <v>4.3129999999999997</v>
+        <v>4.3196399999999997</v>
       </c>
       <c r="O14" s="8">
-        <v>4.3128099999999998</v>
+        <v>4.3190200000000001</v>
       </c>
       <c r="P14" s="9">
-        <v>1.1E-4</v>
+        <v>4.8999999999999998E-4</v>
       </c>
       <c r="Q14" s="18">
-        <v>7.1620200000000001</v>
+        <v>6.9912599999999996</v>
       </c>
       <c r="R14" s="8">
-        <v>7.1785699999999997</v>
+        <v>7.0698600000000003</v>
       </c>
       <c r="S14" s="8">
-        <v>7.1782000000000004</v>
+        <v>6.9944800000000003</v>
       </c>
       <c r="T14" s="9">
-        <v>1.65E-3</v>
+        <v>8.9700000000000005E-3</v>
       </c>
     </row>
     <row r="15" spans="2:20" ht="15.75" thickBot="1">
@@ -3604,52 +4628,52 @@
         <v>250</v>
       </c>
       <c r="E15" s="24">
-        <v>3.7057000000000002</v>
+        <v>5.2709999999999999</v>
       </c>
       <c r="F15" s="25">
-        <v>3.7167400000000002</v>
+        <v>5.2712700000000003</v>
       </c>
       <c r="G15" s="25">
-        <v>3.7160299999999999</v>
+        <v>5.2711800000000002</v>
       </c>
       <c r="H15" s="26">
-        <v>2.7200000000000002E-3</v>
+        <v>1.2E-4</v>
       </c>
       <c r="I15" s="27">
-        <v>1.31332</v>
+        <v>1.2245699999999999</v>
       </c>
       <c r="J15" s="25">
-        <v>1.31429</v>
+        <v>1.2245699999999999</v>
       </c>
       <c r="K15" s="25">
-        <v>1.3133600000000001</v>
+        <v>1.2245699999999999</v>
       </c>
       <c r="L15" s="28">
-        <v>9.0000000000000006E-5</v>
+        <v>0</v>
       </c>
       <c r="M15" s="24">
-        <v>4.3128900000000003</v>
+        <v>4.3048400000000004</v>
       </c>
       <c r="N15" s="25">
-        <v>4.3129400000000002</v>
+        <v>4.7384599999999999</v>
       </c>
       <c r="O15" s="25">
-        <v>4.3129400000000002</v>
+        <v>4.3083</v>
       </c>
       <c r="P15" s="26">
-        <v>1.0000000000000001E-5</v>
+        <v>3.3680000000000002E-2</v>
       </c>
       <c r="Q15" s="27">
-        <v>7.0358900000000002</v>
+        <v>6.9982199999999999</v>
       </c>
       <c r="R15" s="25">
-        <v>7.0358900000000002</v>
+        <v>7.1138000000000003</v>
       </c>
       <c r="S15" s="25">
-        <v>7.0358900000000002</v>
+        <v>7.0000400000000003</v>
       </c>
       <c r="T15" s="26">
-        <v>0</v>
+        <v>1.001E-2</v>
       </c>
     </row>
     <row r="16" spans="2:20">
@@ -3659,52 +4683,52 @@
         <v>20</v>
       </c>
       <c r="E16" s="4">
-        <v>4.3588399999999998</v>
+        <v>4.5548799999999998</v>
       </c>
       <c r="F16" s="5">
-        <v>5.0280899999999997</v>
+        <v>5.7711699999999997</v>
       </c>
       <c r="G16" s="5">
-        <v>4.6608599999999996</v>
+        <v>4.9250999999999996</v>
       </c>
       <c r="H16" s="6">
-        <v>0.12554000000000001</v>
+        <v>0.23702000000000001</v>
       </c>
       <c r="I16" s="17">
-        <v>1.4201299999999999</v>
+        <v>1.4138999999999999</v>
       </c>
       <c r="J16" s="5">
-        <v>1.7423999999999999</v>
+        <v>1.6192299999999999</v>
       </c>
       <c r="K16" s="5">
-        <v>1.56551</v>
+        <v>1.49352</v>
       </c>
       <c r="L16" s="21">
-        <v>5.0389999999999997E-2</v>
+        <v>3.8129999999999997E-2</v>
       </c>
       <c r="M16" s="4">
-        <v>4.3309800000000003</v>
+        <v>4.3350200000000001</v>
       </c>
       <c r="N16" s="5">
-        <v>5.7066999999999997</v>
+        <v>4.9478600000000004</v>
       </c>
       <c r="O16" s="5">
-        <v>4.8270400000000002</v>
+        <v>4.5494500000000002</v>
       </c>
       <c r="P16" s="6">
-        <v>0.29448000000000002</v>
+        <v>0.15029999999999999</v>
       </c>
       <c r="Q16" s="17">
-        <v>7.1901200000000003</v>
+        <v>7.1561000000000003</v>
       </c>
       <c r="R16" s="5">
-        <v>7.5093300000000003</v>
+        <v>7.4490299999999996</v>
       </c>
       <c r="S16" s="5">
-        <v>7.2800700000000003</v>
+        <v>7.2811500000000002</v>
       </c>
       <c r="T16" s="6">
-        <v>6.5329999999999999E-2</v>
+        <v>5.0410000000000003E-2</v>
       </c>
     </row>
     <row r="17" spans="2:20">
@@ -3714,52 +4738,52 @@
         <v>50</v>
       </c>
       <c r="E17" s="7">
-        <v>3.8504100000000001</v>
+        <v>3.76152</v>
       </c>
       <c r="F17" s="8">
-        <v>3.9430100000000001</v>
+        <v>3.77624</v>
       </c>
       <c r="G17" s="8">
-        <v>3.8899599999999999</v>
+        <v>3.7717000000000001</v>
       </c>
       <c r="H17" s="9">
-        <v>3.0810000000000001E-2</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="I17" s="18">
-        <v>1.2259199999999999</v>
+        <v>1.2660800000000001</v>
       </c>
       <c r="J17" s="8">
-        <v>1.2470699999999999</v>
+        <v>1.28366</v>
       </c>
       <c r="K17" s="8">
-        <v>1.2396</v>
+        <v>1.27989</v>
       </c>
       <c r="L17" s="22">
-        <v>3.14E-3</v>
+        <v>2.6700000000000001E-3</v>
       </c>
       <c r="M17" s="7">
-        <v>4.3150399999999998</v>
+        <v>4.3115800000000002</v>
       </c>
       <c r="N17" s="8">
-        <v>4.3157399999999999</v>
+        <v>4.31271</v>
       </c>
       <c r="O17" s="8">
-        <v>4.3155200000000002</v>
+        <v>4.3123399999999998</v>
       </c>
       <c r="P17" s="9">
-        <v>1.2E-4</v>
+        <v>2.9E-4</v>
       </c>
       <c r="Q17" s="18">
-        <v>6.9926599999999999</v>
+        <v>6.9918500000000003</v>
       </c>
       <c r="R17" s="8">
-        <v>7.0074100000000001</v>
+        <v>7.0004</v>
       </c>
       <c r="S17" s="8">
-        <v>7.0008900000000001</v>
+        <v>6.9952899999999998</v>
       </c>
       <c r="T17" s="9">
-        <v>2.6700000000000001E-3</v>
+        <v>2.8999999999999998E-3</v>
       </c>
     </row>
     <row r="18" spans="2:20">
@@ -3771,52 +4795,52 @@
         <v>100</v>
       </c>
       <c r="E18" s="7">
-        <v>3.6245599999999998</v>
+        <v>4.27067</v>
       </c>
       <c r="F18" s="8">
-        <v>3.62608</v>
+        <v>4.3313499999999996</v>
       </c>
       <c r="G18" s="8">
-        <v>3.62588</v>
+        <v>4.29087</v>
       </c>
       <c r="H18" s="9">
-        <v>1.6000000000000001E-4</v>
+        <v>9.0200000000000002E-3</v>
       </c>
       <c r="I18" s="18">
-        <v>1.4495800000000001</v>
+        <v>1.34781</v>
       </c>
       <c r="J18" s="8">
-        <v>1.4523200000000001</v>
+        <v>1.35429</v>
       </c>
       <c r="K18" s="8">
-        <v>1.45007</v>
+        <v>1.3523400000000001</v>
       </c>
       <c r="L18" s="22">
-        <v>3.1E-4</v>
+        <v>8.4000000000000003E-4</v>
       </c>
       <c r="M18" s="7">
-        <v>4.3099600000000002</v>
+        <v>4.3172100000000002</v>
       </c>
       <c r="N18" s="8">
-        <v>4.3102799999999997</v>
+        <v>4.31724</v>
       </c>
       <c r="O18" s="8">
-        <v>4.3101599999999998</v>
+        <v>4.3172300000000003</v>
       </c>
       <c r="P18" s="9">
-        <v>1.6000000000000001E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q18" s="18">
-        <v>6.97682</v>
+        <v>7.0212399999999997</v>
       </c>
       <c r="R18" s="8">
-        <v>7.0294299999999996</v>
+        <v>7.0631199999999996</v>
       </c>
       <c r="S18" s="8">
-        <v>6.9791600000000003</v>
+        <v>7.0240900000000002</v>
       </c>
       <c r="T18" s="9">
-        <v>4.2500000000000003E-3</v>
+        <v>2.49E-3</v>
       </c>
     </row>
     <row r="19" spans="2:20" ht="15.75" thickBot="1">
@@ -3826,52 +4850,52 @@
         <v>250</v>
       </c>
       <c r="E19" s="10">
-        <v>3.7179099999999998</v>
+        <v>3.8198799999999999</v>
       </c>
       <c r="F19" s="11">
-        <v>3.7179199999999999</v>
+        <v>3.8464299999999998</v>
       </c>
       <c r="G19" s="11">
-        <v>3.7179099999999998</v>
+        <v>3.8207300000000002</v>
       </c>
       <c r="H19" s="12">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="I19" s="19">
+        <v>1.2429699999999999</v>
+      </c>
+      <c r="J19" s="11">
+        <v>1.36612</v>
+      </c>
+      <c r="K19" s="11">
+        <v>1.24353</v>
+      </c>
+      <c r="L19" s="23">
+        <v>5.8900000000000003E-3</v>
+      </c>
+      <c r="M19" s="10">
+        <v>4.3050199999999998</v>
+      </c>
+      <c r="N19" s="11">
+        <v>4.3050199999999998</v>
+      </c>
+      <c r="O19" s="11">
+        <v>4.3050199999999998</v>
+      </c>
+      <c r="P19" s="12">
         <v>0</v>
       </c>
-      <c r="I19" s="19">
-        <v>1.1667799999999999</v>
-      </c>
-      <c r="J19" s="11">
-        <v>1.3599000000000001</v>
-      </c>
-      <c r="K19" s="11">
-        <v>1.1691</v>
-      </c>
-      <c r="L19" s="23">
-        <v>1.8870000000000001E-2</v>
-      </c>
-      <c r="M19" s="10">
-        <v>4.3056799999999997</v>
-      </c>
-      <c r="N19" s="11">
-        <v>4.3072999999999997</v>
-      </c>
-      <c r="O19" s="11">
-        <v>4.3056799999999997</v>
-      </c>
-      <c r="P19" s="12">
-        <v>8.0000000000000007E-5</v>
-      </c>
       <c r="Q19" s="19">
-        <v>6.9609100000000002</v>
+        <v>6.9721900000000003</v>
       </c>
       <c r="R19" s="11">
-        <v>6.9610000000000003</v>
+        <v>6.9725999999999999</v>
       </c>
       <c r="S19" s="11">
-        <v>6.9609500000000004</v>
+        <v>6.9725900000000003</v>
       </c>
       <c r="T19" s="12">
-        <v>2.0000000000000002E-5</v>
+        <v>6.0000000000000002E-5</v>
       </c>
     </row>
     <row r="20" spans="2:20">
@@ -3881,52 +4905,52 @@
         <v>20</v>
       </c>
       <c r="E20" s="4">
-        <v>13.11402</v>
+        <v>9.0756899999999998</v>
       </c>
       <c r="F20" s="5">
-        <v>14.225680000000001</v>
+        <v>10.454549999999999</v>
       </c>
       <c r="G20" s="5">
-        <v>13.89715</v>
+        <v>10.198370000000001</v>
       </c>
       <c r="H20" s="6">
-        <v>0.26057000000000002</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="I20" s="17">
-        <v>3.7111999999999998</v>
+        <v>2.6342599999999998</v>
       </c>
       <c r="J20" s="5">
-        <v>3.9493800000000001</v>
+        <v>2.9765600000000001</v>
       </c>
       <c r="K20" s="5">
-        <v>3.9025500000000002</v>
+        <v>2.9416199999999999</v>
       </c>
       <c r="L20" s="21">
-        <v>4.582E-2</v>
+        <v>4.8009999999999997E-2</v>
       </c>
       <c r="M20" s="4">
-        <v>13.5825</v>
+        <v>12.80359</v>
       </c>
       <c r="N20" s="5">
-        <v>15.13381</v>
+        <v>13.045529999999999</v>
       </c>
       <c r="O20" s="5">
-        <v>14.17468</v>
+        <v>12.81423</v>
       </c>
       <c r="P20" s="6">
-        <v>0.49</v>
+        <v>3.798E-2</v>
       </c>
       <c r="Q20" s="17">
-        <v>9.5425799999999992</v>
+        <v>10.79734</v>
       </c>
       <c r="R20" s="5">
-        <v>10.02932</v>
+        <v>11.26238</v>
       </c>
       <c r="S20" s="5">
-        <v>9.8751499999999997</v>
+        <v>10.98803</v>
       </c>
       <c r="T20" s="6">
-        <v>0.1545</v>
+        <v>0.11971</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -3936,52 +4960,52 @@
         <v>50</v>
       </c>
       <c r="E21" s="7">
-        <v>9.8553800000000003</v>
+        <v>9.1212199999999992</v>
       </c>
       <c r="F21" s="8">
-        <v>10.385149999999999</v>
+        <v>9.36416</v>
       </c>
       <c r="G21" s="8">
-        <v>10.2881</v>
+        <v>9.2667699999999993</v>
       </c>
       <c r="H21" s="9">
-        <v>0.14477000000000001</v>
+        <v>0.11878</v>
       </c>
       <c r="I21" s="18">
-        <v>2.6593499999999999</v>
+        <v>2.8495499999999998</v>
       </c>
       <c r="J21" s="8">
-        <v>2.8014299999999999</v>
+        <v>3.0063900000000001</v>
       </c>
       <c r="K21" s="8">
-        <v>2.7805900000000001</v>
+        <v>2.86225</v>
       </c>
       <c r="L21" s="22">
-        <v>3.6819999999999999E-2</v>
+        <v>2.3630000000000002E-2</v>
       </c>
       <c r="M21" s="7">
-        <v>7.5010199999999996</v>
+        <v>9.1826399999999992</v>
       </c>
       <c r="N21" s="8">
-        <v>8.2893699999999999</v>
+        <v>9.1835400000000007</v>
       </c>
       <c r="O21" s="8">
-        <v>8.1006900000000002</v>
+        <v>9.1834799999999994</v>
       </c>
       <c r="P21" s="9">
-        <v>0.23411999999999999</v>
+        <v>1.2999999999999999E-4</v>
       </c>
       <c r="Q21" s="18">
-        <v>8.3377700000000008</v>
+        <v>8.8634199999999996</v>
       </c>
       <c r="R21" s="8">
-        <v>8.5512800000000002</v>
+        <v>8.9470200000000002</v>
       </c>
       <c r="S21" s="8">
-        <v>8.4613300000000002</v>
+        <v>8.9055599999999995</v>
       </c>
       <c r="T21" s="9">
-        <v>4.9450000000000001E-2</v>
+        <v>2.4209999999999999E-2</v>
       </c>
     </row>
     <row r="22" spans="2:20">
@@ -3993,52 +5017,52 @@
         <v>100</v>
       </c>
       <c r="E22" s="7">
-        <v>7.6700200000000001</v>
+        <v>7.3029799999999998</v>
       </c>
       <c r="F22" s="8">
-        <v>7.8457499999999998</v>
+        <v>7.6247600000000002</v>
       </c>
       <c r="G22" s="8">
-        <v>7.7813499999999998</v>
+        <v>7.5655000000000001</v>
       </c>
       <c r="H22" s="9">
-        <v>5.7750000000000003E-2</v>
+        <v>0.11589000000000001</v>
       </c>
       <c r="I22" s="18">
-        <v>2.5218600000000002</v>
+        <v>2.4167299999999998</v>
       </c>
       <c r="J22" s="8">
-        <v>2.5686599999999999</v>
+        <v>2.8454899999999999</v>
       </c>
       <c r="K22" s="8">
-        <v>2.56582</v>
+        <v>2.4699499999999999</v>
       </c>
       <c r="L22" s="22">
-        <v>1.111E-2</v>
+        <v>6.565E-2</v>
       </c>
       <c r="M22" s="7">
-        <v>8.5473400000000002</v>
+        <v>7.2934000000000001</v>
       </c>
       <c r="N22" s="8">
-        <v>9.7410899999999998</v>
+        <v>7.3037099999999997</v>
       </c>
       <c r="O22" s="8">
-        <v>8.5778700000000008</v>
+        <v>7.3030900000000001</v>
       </c>
       <c r="P22" s="9">
-        <v>0.16838</v>
+        <v>2.4499999999999999E-3</v>
       </c>
       <c r="Q22" s="18">
-        <v>8.4149399999999996</v>
+        <v>8.4125099999999993</v>
       </c>
       <c r="R22" s="8">
-        <v>8.4149399999999996</v>
+        <v>8.4358900000000006</v>
       </c>
       <c r="S22" s="8">
-        <v>8.4149399999999996</v>
+        <v>8.4162499999999998</v>
       </c>
       <c r="T22" s="9">
-        <v>0</v>
+        <v>8.5699999999999995E-3</v>
       </c>
     </row>
     <row r="23" spans="2:20" ht="15.75" thickBot="1">
@@ -4048,52 +5072,52 @@
         <v>250</v>
       </c>
       <c r="E23" s="24">
-        <v>7.4081099999999998</v>
+        <v>5.9764600000000003</v>
       </c>
       <c r="F23" s="25">
-        <v>7.4361899999999999</v>
+        <v>5.9764600000000003</v>
       </c>
       <c r="G23" s="25">
-        <v>7.4095000000000004</v>
+        <v>5.9764600000000003</v>
       </c>
       <c r="H23" s="26">
-        <v>5.5500000000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="I23" s="27">
-        <v>1.6568000000000001</v>
+        <v>1.9069100000000001</v>
       </c>
       <c r="J23" s="25">
-        <v>1.6607700000000001</v>
+        <v>1.91489</v>
       </c>
       <c r="K23" s="25">
-        <v>1.66045</v>
+        <v>1.91225</v>
       </c>
       <c r="L23" s="28">
-        <v>1.08E-3</v>
+        <v>3.6800000000000001E-3</v>
       </c>
       <c r="M23" s="24">
-        <v>5.4358700000000004</v>
+        <v>6.5014799999999999</v>
       </c>
       <c r="N23" s="25">
-        <v>5.9384699999999997</v>
+        <v>6.5014799999999999</v>
       </c>
       <c r="O23" s="25">
-        <v>5.4543999999999997</v>
+        <v>6.5014799999999999</v>
       </c>
       <c r="P23" s="26">
-        <v>7.2520000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="Q23" s="27">
-        <v>8.2914700000000003</v>
+        <v>7.6032700000000002</v>
       </c>
       <c r="R23" s="25">
-        <v>8.4804399999999998</v>
+        <v>7.6035899999999996</v>
       </c>
       <c r="S23" s="25">
-        <v>8.3052100000000006</v>
+        <v>7.6035500000000003</v>
       </c>
       <c r="T23" s="26">
-        <v>3.0110000000000001E-2</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="24" spans="2:20">
@@ -4103,52 +5127,52 @@
         <v>20</v>
       </c>
       <c r="E24" s="4">
-        <v>10.116009999999999</v>
+        <v>10.61992</v>
       </c>
       <c r="F24" s="5">
-        <v>11.531470000000001</v>
+        <v>12.738899999999999</v>
       </c>
       <c r="G24" s="5">
-        <v>10.92008</v>
+        <v>11.5886</v>
       </c>
       <c r="H24" s="6">
-        <v>0.26543</v>
+        <v>0.42786999999999997</v>
       </c>
       <c r="I24" s="17">
-        <v>2.72715</v>
+        <v>4.0296000000000003</v>
       </c>
       <c r="J24" s="5">
-        <v>3.2406999999999999</v>
+        <v>4.4671000000000003</v>
       </c>
       <c r="K24" s="5">
-        <v>3.0016099999999999</v>
+        <v>4.31264</v>
       </c>
       <c r="L24" s="21">
-        <v>0.12164999999999999</v>
+        <v>0.11179</v>
       </c>
       <c r="M24" s="4">
-        <v>10.555680000000001</v>
+        <v>9.78505</v>
       </c>
       <c r="N24" s="5">
-        <v>12.19007</v>
+        <v>10.729150000000001</v>
       </c>
       <c r="O24" s="5">
-        <v>11.24405</v>
+        <v>10.23593</v>
       </c>
       <c r="P24" s="6">
-        <v>0.36046</v>
+        <v>0.27393000000000001</v>
       </c>
       <c r="Q24" s="17">
-        <v>8.7826799999999992</v>
+        <v>8.9058299999999999</v>
       </c>
       <c r="R24" s="5">
-        <v>9.5688700000000004</v>
+        <v>9.5466800000000003</v>
       </c>
       <c r="S24" s="5">
-        <v>9.2835999999999999</v>
+        <v>9.2888900000000003</v>
       </c>
       <c r="T24" s="6">
-        <v>0.15135000000000001</v>
+        <v>0.13100999999999999</v>
       </c>
     </row>
     <row r="25" spans="2:20">
@@ -4158,52 +5182,52 @@
         <v>50</v>
       </c>
       <c r="E25" s="7">
-        <v>6.8666900000000002</v>
+        <v>7.8502299999999998</v>
       </c>
       <c r="F25" s="8">
-        <v>7.2865500000000001</v>
+        <v>8.1639499999999998</v>
       </c>
       <c r="G25" s="8">
-        <v>6.9846199999999996</v>
+        <v>8.01356</v>
       </c>
       <c r="H25" s="9">
-        <v>0.10874</v>
+        <v>5.8860000000000003E-2</v>
       </c>
       <c r="I25" s="18">
-        <v>2.6957300000000002</v>
+        <v>2.28613</v>
       </c>
       <c r="J25" s="8">
-        <v>2.9836299999999998</v>
+        <v>2.3172600000000001</v>
       </c>
       <c r="K25" s="8">
-        <v>2.7339899999999999</v>
+        <v>2.3158099999999999</v>
       </c>
       <c r="L25" s="22">
-        <v>4.5569999999999999E-2</v>
+        <v>3.5300000000000002E-3</v>
       </c>
       <c r="M25" s="7">
-        <v>6.95397</v>
+        <v>7.7179099999999998</v>
       </c>
       <c r="N25" s="8">
-        <v>7.0608199999999997</v>
+        <v>8.7057599999999997</v>
       </c>
       <c r="O25" s="8">
-        <v>7.0415299999999998</v>
+        <v>8.3021999999999991</v>
       </c>
       <c r="P25" s="9">
-        <v>2.5250000000000002E-2</v>
+        <v>0.23150999999999999</v>
       </c>
       <c r="Q25" s="18">
-        <v>8.03796</v>
+        <v>7.5380700000000003</v>
       </c>
       <c r="R25" s="8">
-        <v>8.3185699999999994</v>
+        <v>7.6432599999999997</v>
       </c>
       <c r="S25" s="8">
-        <v>8.0726099999999992</v>
+        <v>7.5819900000000002</v>
       </c>
       <c r="T25" s="9">
-        <v>4.2500000000000003E-2</v>
+        <v>1.7399999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="2:20">
@@ -4215,52 +5239,52 @@
         <v>100</v>
       </c>
       <c r="E26" s="7">
-        <v>7.5544099999999998</v>
+        <v>5.6490900000000002</v>
       </c>
       <c r="F26" s="8">
-        <v>7.5766600000000004</v>
+        <v>5.7420299999999997</v>
       </c>
       <c r="G26" s="8">
-        <v>7.5752300000000004</v>
+        <v>5.6785100000000002</v>
       </c>
       <c r="H26" s="9">
-        <v>4.7499999999999999E-3</v>
+        <v>2.0209999999999999E-2</v>
       </c>
       <c r="I26" s="18">
-        <v>2.1079599999999998</v>
+        <v>1.9473</v>
       </c>
       <c r="J26" s="8">
-        <v>2.1369500000000001</v>
+        <v>1.9612799999999999</v>
       </c>
       <c r="K26" s="8">
-        <v>2.1237499999999998</v>
+        <v>1.9565999999999999</v>
       </c>
       <c r="L26" s="22">
-        <v>1.4250000000000001E-2</v>
+        <v>6.2199999999999998E-3</v>
       </c>
       <c r="M26" s="7">
-        <v>7.4010899999999999</v>
+        <v>5.9542099999999998</v>
       </c>
       <c r="N26" s="8">
-        <v>7.5889100000000003</v>
+        <v>7.0495599999999996</v>
       </c>
       <c r="O26" s="8">
-        <v>7.5030400000000004</v>
+        <v>6.0245899999999999</v>
       </c>
       <c r="P26" s="9">
-        <v>4.7669999999999997E-2</v>
+        <v>0.12472</v>
       </c>
       <c r="Q26" s="18">
-        <v>7.5428300000000004</v>
+        <v>7.7270399999999997</v>
       </c>
       <c r="R26" s="8">
-        <v>7.5615600000000001</v>
+        <v>8.2134999999999998</v>
       </c>
       <c r="S26" s="8">
-        <v>7.55586</v>
+        <v>7.7452300000000003</v>
       </c>
       <c r="T26" s="9">
-        <v>5.9199999999999999E-3</v>
+        <v>6.4360000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="2:20" ht="15.75" thickBot="1">
@@ -4272,52 +5296,52 @@
         <v>250</v>
       </c>
       <c r="E27" s="24">
-        <v>6.7403399999999998</v>
+        <v>5.8242900000000004</v>
       </c>
       <c r="F27" s="25">
-        <v>6.8346200000000001</v>
+        <v>6.1620400000000002</v>
       </c>
       <c r="G27" s="25">
-        <v>6.8335900000000001</v>
+        <v>5.8301499999999997</v>
       </c>
       <c r="H27" s="26">
-        <v>9.3699999999999999E-3</v>
+        <v>3.8100000000000002E-2</v>
       </c>
       <c r="I27" s="27">
-        <v>1.8139700000000001</v>
+        <v>1.68953</v>
       </c>
       <c r="J27" s="25">
-        <v>1.8209200000000001</v>
+        <v>1.7785299999999999</v>
       </c>
       <c r="K27" s="25">
-        <v>1.81488</v>
+        <v>1.69157</v>
       </c>
       <c r="L27" s="28">
-        <v>2.15E-3</v>
+        <v>1.1939999999999999E-2</v>
       </c>
       <c r="M27" s="24">
-        <v>5.3483799999999997</v>
+        <v>5.3445799999999997</v>
       </c>
       <c r="N27" s="25">
-        <v>5.4207400000000003</v>
+        <v>5.3507699999999998</v>
       </c>
       <c r="O27" s="25">
-        <v>5.40916</v>
+        <v>5.3489199999999997</v>
       </c>
       <c r="P27" s="26">
-        <v>2.6530000000000001E-2</v>
+        <v>2.6900000000000001E-3</v>
       </c>
       <c r="Q27" s="27">
-        <v>7.5435100000000004</v>
+        <v>7.32986</v>
       </c>
       <c r="R27" s="25">
-        <v>7.5871700000000004</v>
+        <v>7.3303399999999996</v>
       </c>
       <c r="S27" s="25">
-        <v>7.5456899999999996</v>
+        <v>7.33</v>
       </c>
       <c r="T27" s="26">
-        <v>6.1599999999999997E-3</v>
+        <v>2.2000000000000001E-4</v>
       </c>
     </row>
     <row r="28" spans="2:20">
@@ -4327,52 +5351,52 @@
         <v>20</v>
       </c>
       <c r="E28" s="4">
-        <v>8.6103799999999993</v>
+        <v>8.2211999999999996</v>
       </c>
       <c r="F28" s="5">
-        <v>11.279310000000001</v>
+        <v>10.31922</v>
       </c>
       <c r="G28" s="5">
-        <v>9.8199500000000004</v>
+        <v>9.3099299999999996</v>
       </c>
       <c r="H28" s="6">
-        <v>0.60516999999999999</v>
+        <v>0.41833999999999999</v>
       </c>
       <c r="I28" s="17">
-        <v>2.7313100000000001</v>
+        <v>2.4380199999999999</v>
       </c>
       <c r="J28" s="5">
-        <v>3.5126599999999999</v>
+        <v>3.2243400000000002</v>
       </c>
       <c r="K28" s="5">
-        <v>3.1707100000000001</v>
+        <v>2.8068399999999998</v>
       </c>
       <c r="L28" s="21">
-        <v>0.16395000000000001</v>
+        <v>0.17865</v>
       </c>
       <c r="M28" s="4">
-        <v>8.65564</v>
+        <v>8.7647899999999996</v>
       </c>
       <c r="N28" s="5">
-        <v>10.55237</v>
+        <v>11.577489999999999</v>
       </c>
       <c r="O28" s="5">
-        <v>9.8421099999999999</v>
+        <v>9.7848799999999994</v>
       </c>
       <c r="P28" s="6">
-        <v>0.32677</v>
+        <v>0.68598000000000003</v>
       </c>
       <c r="Q28" s="17">
-        <v>9.1842699999999997</v>
+        <v>8.2527000000000008</v>
       </c>
       <c r="R28" s="5">
-        <v>9.86233</v>
+        <v>9.1449099999999994</v>
       </c>
       <c r="S28" s="5">
-        <v>9.5302100000000003</v>
+        <v>8.6752000000000002</v>
       </c>
       <c r="T28" s="6">
-        <v>0.16785</v>
+        <v>0.21407999999999999</v>
       </c>
     </row>
     <row r="29" spans="2:20">
@@ -4382,52 +5406,52 @@
         <v>50</v>
       </c>
       <c r="E29" s="7">
-        <v>6.7534000000000001</v>
+        <v>6.92971</v>
       </c>
       <c r="F29" s="8">
-        <v>6.8676899999999996</v>
+        <v>7.3562000000000003</v>
       </c>
       <c r="G29" s="8">
-        <v>6.7742000000000004</v>
+        <v>7.1185900000000002</v>
       </c>
       <c r="H29" s="9">
-        <v>2.7560000000000001E-2</v>
+        <v>7.9380000000000006E-2</v>
       </c>
       <c r="I29" s="18">
-        <v>2.0889700000000002</v>
+        <v>2.0440100000000001</v>
       </c>
       <c r="J29" s="8">
-        <v>2.4012099999999998</v>
+        <v>2.1782300000000001</v>
       </c>
       <c r="K29" s="8">
-        <v>2.29067</v>
+        <v>2.1103299999999998</v>
       </c>
       <c r="L29" s="22">
-        <v>7.1859999999999993E-2</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="M29" s="7">
-        <v>7.2609700000000004</v>
+        <v>6.5831</v>
       </c>
       <c r="N29" s="8">
-        <v>7.5395399999999997</v>
+        <v>7.3029900000000003</v>
       </c>
       <c r="O29" s="8">
-        <v>7.3803900000000002</v>
+        <v>6.8995100000000003</v>
       </c>
       <c r="P29" s="9">
-        <v>7.4740000000000001E-2</v>
+        <v>0.12941</v>
       </c>
       <c r="Q29" s="18">
-        <v>7.4215999999999998</v>
+        <v>7.7490699999999997</v>
       </c>
       <c r="R29" s="8">
-        <v>7.50101</v>
+        <v>7.8490700000000002</v>
       </c>
       <c r="S29" s="8">
-        <v>7.4437300000000004</v>
+        <v>7.7774599999999996</v>
       </c>
       <c r="T29" s="9">
-        <v>1.8519999999999998E-2</v>
+        <v>1.7590000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="2:20">
@@ -4439,52 +5463,52 @@
         <v>100</v>
       </c>
       <c r="E30" s="7">
-        <v>6.2360300000000004</v>
+        <v>6.1019199999999998</v>
       </c>
       <c r="F30" s="8">
-        <v>6.2559899999999997</v>
+        <v>6.4554499999999999</v>
       </c>
       <c r="G30" s="8">
-        <v>6.2544199999999996</v>
+        <v>6.1226200000000004</v>
       </c>
       <c r="H30" s="9">
-        <v>3.0000000000000001E-3</v>
+        <v>3.7929999999999998E-2</v>
       </c>
       <c r="I30" s="18">
-        <v>1.7819199999999999</v>
+        <v>1.8266</v>
       </c>
       <c r="J30" s="8">
-        <v>1.83507</v>
+        <v>1.8986000000000001</v>
       </c>
       <c r="K30" s="8">
-        <v>1.80559</v>
+        <v>1.83283</v>
       </c>
       <c r="L30" s="22">
-        <v>1.1509999999999999E-2</v>
+        <v>1.018E-2</v>
       </c>
       <c r="M30" s="7">
-        <v>6.5736600000000003</v>
+        <v>5.9592400000000003</v>
       </c>
       <c r="N30" s="8">
-        <v>7.1259499999999996</v>
+        <v>5.9607099999999997</v>
       </c>
       <c r="O30" s="8">
-        <v>6.6342600000000003</v>
+        <v>5.9602700000000004</v>
       </c>
       <c r="P30" s="9">
-        <v>5.5550000000000002E-2</v>
+        <v>5.5000000000000003E-4</v>
       </c>
       <c r="Q30" s="18">
-        <v>7.4658300000000004</v>
+        <v>7.3248300000000004</v>
       </c>
       <c r="R30" s="8">
-        <v>7.5032899999999998</v>
+        <v>7.3891999999999998</v>
       </c>
       <c r="S30" s="8">
-        <v>7.4783299999999997</v>
+        <v>7.3323700000000001</v>
       </c>
       <c r="T30" s="9">
-        <v>6.6400000000000001E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1">
@@ -4494,52 +5518,52 @@
         <v>250</v>
       </c>
       <c r="E31" s="24">
-        <v>4.8987400000000001</v>
+        <v>5.2433800000000002</v>
       </c>
       <c r="F31" s="25">
-        <v>4.9245799999999997</v>
+        <v>5.2536199999999997</v>
       </c>
       <c r="G31" s="25">
-        <v>4.9000199999999996</v>
+        <v>5.2434599999999998</v>
       </c>
       <c r="H31" s="26">
-        <v>1.75E-3</v>
+        <v>7.2000000000000005E-4</v>
       </c>
       <c r="I31" s="27">
-        <v>1.9707399999999999</v>
+        <v>1.8105899999999999</v>
       </c>
       <c r="J31" s="25">
-        <v>2.0200999999999998</v>
+        <v>1.8225100000000001</v>
       </c>
       <c r="K31" s="25">
-        <v>1.9710099999999999</v>
+        <v>1.8220499999999999</v>
       </c>
       <c r="L31" s="28">
-        <v>3.5000000000000001E-3</v>
+        <v>1.6199999999999999E-3</v>
       </c>
       <c r="M31" s="24">
-        <v>5.2103099999999998</v>
+        <v>6.0563700000000003</v>
       </c>
       <c r="N31" s="25">
-        <v>5.2278700000000002</v>
+        <v>6.0563700000000003</v>
       </c>
       <c r="O31" s="25">
-        <v>5.2126900000000003</v>
+        <v>6.0563700000000003</v>
       </c>
       <c r="P31" s="26">
-        <v>3.49E-3</v>
+        <v>0</v>
       </c>
       <c r="Q31" s="27">
-        <v>7.6778500000000003</v>
+        <v>7.2400900000000004</v>
       </c>
       <c r="R31" s="25">
-        <v>7.68546</v>
+        <v>7.2403399999999998</v>
       </c>
       <c r="S31" s="25">
-        <v>7.6780999999999997</v>
+        <v>7.24017</v>
       </c>
       <c r="T31" s="26">
-        <v>7.5000000000000002E-4</v>
+        <v>1.2E-4</v>
       </c>
     </row>
     <row r="32" spans="2:20">
@@ -4549,52 +5573,52 @@
         <v>20</v>
       </c>
       <c r="E32" s="4">
-        <v>8.2036499999999997</v>
+        <v>7.4524499999999998</v>
       </c>
       <c r="F32" s="5">
-        <v>11.4236</v>
+        <v>9.7545800000000007</v>
       </c>
       <c r="G32" s="5">
-        <v>9.8218399999999999</v>
+        <v>8.7319300000000002</v>
       </c>
       <c r="H32" s="6">
-        <v>0.64415</v>
+        <v>0.43117</v>
       </c>
       <c r="I32" s="17">
-        <v>2.7564600000000001</v>
+        <v>2.6806999999999999</v>
       </c>
       <c r="J32" s="5">
-        <v>4.0212000000000003</v>
+        <v>3.9073799999999999</v>
       </c>
       <c r="K32" s="5">
-        <v>3.3329499999999999</v>
+        <v>3.2980399999999999</v>
       </c>
       <c r="L32" s="21">
-        <v>0.27100000000000002</v>
+        <v>0.25689000000000001</v>
       </c>
       <c r="M32" s="4">
-        <v>7.7775100000000004</v>
+        <v>8.1683199999999996</v>
       </c>
       <c r="N32" s="5">
-        <v>10.847020000000001</v>
+        <v>11.559150000000001</v>
       </c>
       <c r="O32" s="5">
-        <v>9.3369400000000002</v>
+        <v>9.7970199999999998</v>
       </c>
       <c r="P32" s="6">
-        <v>0.61967000000000005</v>
+        <v>0.75019000000000002</v>
       </c>
       <c r="Q32" s="17">
-        <v>7.9524400000000002</v>
+        <v>8.2269799999999993</v>
       </c>
       <c r="R32" s="5">
-        <v>9.0039499999999997</v>
+        <v>9.2728400000000004</v>
       </c>
       <c r="S32" s="5">
-        <v>8.5348400000000009</v>
+        <v>8.7838899999999995</v>
       </c>
       <c r="T32" s="6">
-        <v>0.20607</v>
+        <v>0.21057000000000001</v>
       </c>
     </row>
     <row r="33" spans="2:20">
@@ -4604,52 +5628,52 @@
         <v>50</v>
       </c>
       <c r="E33" s="7">
-        <v>6.3113000000000001</v>
+        <v>5.6317199999999996</v>
       </c>
       <c r="F33" s="8">
-        <v>6.5526900000000001</v>
+        <v>5.7800900000000004</v>
       </c>
       <c r="G33" s="8">
-        <v>6.3933</v>
+        <v>5.7151399999999999</v>
       </c>
       <c r="H33" s="9">
-        <v>5.4350000000000002E-2</v>
+        <v>2.9729999999999999E-2</v>
       </c>
       <c r="I33" s="18">
-        <v>2.20818</v>
+        <v>2.0636700000000001</v>
       </c>
       <c r="J33" s="8">
-        <v>2.3451499999999998</v>
+        <v>2.12642</v>
       </c>
       <c r="K33" s="8">
-        <v>2.2400199999999999</v>
+        <v>2.0792199999999998</v>
       </c>
       <c r="L33" s="22">
-        <v>1.341E-2</v>
+        <v>4.2300000000000003E-3</v>
       </c>
       <c r="M33" s="7">
-        <v>5.2359600000000004</v>
+        <v>5.9617599999999999</v>
       </c>
       <c r="N33" s="8">
-        <v>5.5154399999999999</v>
+        <v>6.1757999999999997</v>
       </c>
       <c r="O33" s="8">
-        <v>5.3890599999999997</v>
+        <v>6.0216200000000004</v>
       </c>
       <c r="P33" s="9">
-        <v>5.3699999999999998E-2</v>
+        <v>4.061E-2</v>
       </c>
       <c r="Q33" s="18">
-        <v>7.6689499999999997</v>
+        <v>7.48081</v>
       </c>
       <c r="R33" s="8">
-        <v>7.7345499999999996</v>
+        <v>7.5207100000000002</v>
       </c>
       <c r="S33" s="8">
-        <v>7.7035900000000002</v>
+        <v>7.5099299999999998</v>
       </c>
       <c r="T33" s="9">
-        <v>8.9899999999999997E-3</v>
+        <v>4.5199999999999997E-3</v>
       </c>
     </row>
     <row r="34" spans="2:20">
@@ -4661,52 +5685,52 @@
         <v>100</v>
       </c>
       <c r="E34" s="7">
-        <v>4.7403199999999996</v>
+        <v>5.8579800000000004</v>
       </c>
       <c r="F34" s="8">
-        <v>4.8021500000000001</v>
+        <v>5.9027000000000003</v>
       </c>
       <c r="G34" s="8">
-        <v>4.7831099999999998</v>
+        <v>5.8866199999999997</v>
       </c>
       <c r="H34" s="9">
-        <v>1.49E-2</v>
+        <v>5.7400000000000003E-3</v>
       </c>
       <c r="I34" s="18">
-        <v>1.4878800000000001</v>
+        <v>1.51162</v>
       </c>
       <c r="J34" s="8">
-        <v>1.53451</v>
+        <v>1.57345</v>
       </c>
       <c r="K34" s="8">
-        <v>1.48902</v>
+        <v>1.51572</v>
       </c>
       <c r="L34" s="22">
-        <v>3.81E-3</v>
+        <v>4.3800000000000002E-3</v>
       </c>
       <c r="M34" s="7">
-        <v>4.8400499999999997</v>
+        <v>5.3660500000000004</v>
       </c>
       <c r="N34" s="8">
-        <v>5.0527600000000001</v>
+        <v>5.4727300000000003</v>
       </c>
       <c r="O34" s="8">
-        <v>4.8859599999999999</v>
+        <v>5.4108599999999996</v>
       </c>
       <c r="P34" s="9">
-        <v>1.499E-2</v>
+        <v>2.188E-2</v>
       </c>
       <c r="Q34" s="18">
-        <v>7.3379700000000003</v>
+        <v>7.4158400000000002</v>
       </c>
       <c r="R34" s="8">
-        <v>7.34565</v>
+        <v>7.4369899999999998</v>
       </c>
       <c r="S34" s="8">
-        <v>7.3425799999999999</v>
+        <v>7.4267799999999999</v>
       </c>
       <c r="T34" s="9">
-        <v>1.4400000000000001E-3</v>
+        <v>4.5100000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="2:20" ht="15.75" thickBot="1">
@@ -4716,52 +5740,52 @@
         <v>250</v>
       </c>
       <c r="E35" s="10">
-        <v>4.7431999999999999</v>
+        <v>4.7567500000000003</v>
       </c>
       <c r="F35" s="11">
-        <v>4.7435</v>
+        <v>4.7960700000000003</v>
       </c>
       <c r="G35" s="11">
-        <v>4.7432299999999996</v>
+        <v>4.7769399999999997</v>
       </c>
       <c r="H35" s="12">
-        <v>1.0000000000000001E-5</v>
+        <v>1.26E-2</v>
       </c>
       <c r="I35" s="19">
-        <v>1.4693799999999999</v>
+        <v>1.43635</v>
       </c>
       <c r="J35" s="11">
-        <v>1.5639099999999999</v>
+        <v>1.44089</v>
       </c>
       <c r="K35" s="11">
-        <v>1.47383</v>
+        <v>1.44049</v>
       </c>
       <c r="L35" s="23">
-        <v>4.1999999999999997E-3</v>
+        <v>7.2999999999999996E-4</v>
       </c>
       <c r="M35" s="10">
-        <v>4.8963700000000001</v>
+        <v>4.3248699999999998</v>
       </c>
       <c r="N35" s="11">
-        <v>5.1132799999999996</v>
+        <v>4.3359399999999999</v>
       </c>
       <c r="O35" s="11">
-        <v>4.92239</v>
+        <v>4.3254700000000001</v>
       </c>
       <c r="P35" s="12">
-        <v>1.2869999999999999E-2</v>
+        <v>5.1000000000000004E-4</v>
       </c>
       <c r="Q35" s="19">
-        <v>7.1223700000000001</v>
+        <v>7.0894199999999996</v>
       </c>
       <c r="R35" s="11">
-        <v>7.1236300000000004</v>
+        <v>7.1201800000000004</v>
       </c>
       <c r="S35" s="11">
-        <v>7.1236100000000002</v>
+        <v>7.0918200000000002</v>
       </c>
       <c r="T35" s="12">
-        <v>1.6000000000000001E-4</v>
+        <v>1.5900000000000001E-3</v>
       </c>
     </row>
     <row r="37" spans="2:20" ht="15.75" thickBot="1"/>

</xml_diff>